<commit_message>
fixed W-band pol position in table
</commit_message>
<xml_diff>
--- a/data/default_biases_warm.xlsx
+++ b/data/default_biases_warm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Biases" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
   <si>
     <t xml:space="preserve">PAR</t>
   </si>
@@ -47,127 +47,127 @@
     <t xml:space="preserve">STRIP17</t>
   </si>
   <si>
+    <t xml:space="preserve">STRIP71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIP63</t>
+  </si>
+  <si>
     <t xml:space="preserve">STRIP78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP76</t>
   </si>
   <si>
     <t xml:space="preserve">STRIP31</t>
@@ -605,13 +605,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -681,16 +681,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BE29"/>
+  <dimension ref="A1:BD29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AR1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BF1" activeCellId="0" sqref="BF1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AW1" activeCellId="0" sqref="AW1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="0" width="8.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1" style="0" width="8.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -790,79 +791,76 @@
       <c r="AF1" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="AH1" s="0" t="s">
+        <v>33</v>
+      </c>
       <c r="AI1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="AP1" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="AQ1" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW1" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="AX1" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="AY1" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="BE1" s="0" t="s">
         <v>55</v>
       </c>
     </row>
@@ -892,7 +890,7 @@
         <v>800</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>800</v>
@@ -916,7 +914,7 @@
         <v>800</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="R2" s="0" t="n">
         <v>800</v>
@@ -940,7 +938,7 @@
         <v>800</v>
       </c>
       <c r="Y2" s="1" t="n">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="Z2" s="0" t="n">
         <v>800</v>
@@ -963,10 +961,10 @@
       <c r="AF2" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AG2" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AH2" s="1" t="n">
+      <c r="AG2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="0" t="n">
         <v>800</v>
       </c>
       <c r="AI2" s="0" t="n">
@@ -987,11 +985,11 @@
       <c r="AN2" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AO2" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AP2" s="2" t="n">
-        <v>0</v>
+      <c r="AO2" s="1" t="n">
+        <v>800</v>
+      </c>
+      <c r="AP2" s="0" t="n">
+        <v>800</v>
       </c>
       <c r="AQ2" s="0" t="n">
         <v>800</v>
@@ -1011,10 +1009,10 @@
       <c r="AV2" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AW2" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AX2" s="1" t="n">
+      <c r="AW2" s="1" t="n">
+        <v>800</v>
+      </c>
+      <c r="AX2" s="0" t="n">
         <v>800</v>
       </c>
       <c r="AY2" s="0" t="n">
@@ -1033,9 +1031,6 @@
         <v>800</v>
       </c>
       <c r="BD2" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="BE2" s="0" t="n">
         <v>800</v>
       </c>
     </row>
@@ -1065,7 +1060,7 @@
         <v>800</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>800</v>
@@ -1113,7 +1108,7 @@
         <v>600</v>
       </c>
       <c r="Y3" s="1" t="n">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="Z3" s="0" t="n">
         <v>800</v>
@@ -1136,10 +1131,10 @@
       <c r="AF3" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AG3" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AH3" s="1" t="n">
+      <c r="AG3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="0" t="n">
         <v>800</v>
       </c>
       <c r="AI3" s="0" t="n">
@@ -1149,46 +1144,46 @@
         <v>800</v>
       </c>
       <c r="AK3" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="AL3" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="AN3" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="AM3" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AN3" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AO3" s="0" t="n">
+      <c r="AO3" s="1" t="n">
         <v>600</v>
       </c>
-      <c r="AP3" s="2" t="n">
-        <v>0</v>
+      <c r="AP3" s="0" t="n">
+        <v>600</v>
       </c>
       <c r="AQ3" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="AR3" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="AS3" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="AR3" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AS3" s="0" t="n">
-        <v>800</v>
-      </c>
       <c r="AT3" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="AU3" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="AV3" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="AW3" s="1" t="n">
         <v>600</v>
       </c>
-      <c r="AU3" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AV3" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AW3" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AX3" s="1" t="n">
-        <v>600</v>
+      <c r="AX3" s="0" t="n">
+        <v>800</v>
       </c>
       <c r="AY3" s="0" t="n">
         <v>800</v>
@@ -1206,9 +1201,6 @@
         <v>800</v>
       </c>
       <c r="BD3" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="BE3" s="0" t="n">
         <v>800</v>
       </c>
     </row>
@@ -1309,11 +1301,11 @@
       <c r="AF4" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AG4" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AH4" s="1" t="n">
-        <v>0</v>
+      <c r="AG4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="0" t="n">
+        <v>800</v>
       </c>
       <c r="AI4" s="0" t="n">
         <v>800</v>
@@ -1333,11 +1325,11 @@
       <c r="AN4" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AO4" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AP4" s="2" t="n">
-        <v>0</v>
+      <c r="AO4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="0" t="n">
+        <v>800</v>
       </c>
       <c r="AQ4" s="0" t="n">
         <v>800</v>
@@ -1357,11 +1349,11 @@
       <c r="AV4" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AW4" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AX4" s="1" t="n">
-        <v>0</v>
+      <c r="AW4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="0" t="n">
+        <v>800</v>
       </c>
       <c r="AY4" s="0" t="n">
         <v>800</v>
@@ -1370,18 +1362,15 @@
         <v>800</v>
       </c>
       <c r="BA4" s="0" t="n">
-        <v>800</v>
+        <v>200</v>
       </c>
       <c r="BB4" s="0" t="n">
-        <v>200</v>
+        <v>800</v>
       </c>
       <c r="BC4" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="BD4" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="BE4" s="0" t="n">
         <v>800</v>
       </c>
     </row>
@@ -1482,11 +1471,11 @@
       <c r="AF5" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AG5" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AH5" s="1" t="n">
-        <v>0</v>
+      <c r="AG5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="0" t="n">
+        <v>800</v>
       </c>
       <c r="AI5" s="0" t="n">
         <v>800</v>
@@ -1506,11 +1495,11 @@
       <c r="AN5" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AO5" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AP5" s="2" t="n">
-        <v>0</v>
+      <c r="AO5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="0" t="n">
+        <v>800</v>
       </c>
       <c r="AQ5" s="0" t="n">
         <v>800</v>
@@ -1530,11 +1519,11 @@
       <c r="AV5" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AW5" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AX5" s="1" t="n">
-        <v>0</v>
+      <c r="AW5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="0" t="n">
+        <v>800</v>
       </c>
       <c r="AY5" s="0" t="n">
         <v>800</v>
@@ -1546,15 +1535,12 @@
         <v>800</v>
       </c>
       <c r="BB5" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="BC5" s="0" t="n">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="BD5" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="BE5" s="0" t="n">
         <v>800</v>
       </c>
     </row>
@@ -1584,7 +1570,7 @@
         <v>800</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>800</v>
@@ -1632,7 +1618,7 @@
         <v>600</v>
       </c>
       <c r="Y6" s="1" t="n">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="Z6" s="0" t="n">
         <v>800</v>
@@ -1655,10 +1641,10 @@
       <c r="AF6" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AG6" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AH6" s="1" t="n">
+      <c r="AG6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="0" t="n">
         <v>800</v>
       </c>
       <c r="AI6" s="0" t="n">
@@ -1679,11 +1665,11 @@
       <c r="AN6" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AO6" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AP6" s="2" t="n">
-        <v>0</v>
+      <c r="AO6" s="1" t="n">
+        <v>600</v>
+      </c>
+      <c r="AP6" s="0" t="n">
+        <v>800</v>
       </c>
       <c r="AQ6" s="0" t="n">
         <v>800</v>
@@ -1703,12 +1689,12 @@
       <c r="AV6" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AW6" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AX6" s="1" t="n">
+      <c r="AW6" s="1" t="n">
         <v>600</v>
       </c>
+      <c r="AX6" s="0" t="n">
+        <v>800</v>
+      </c>
       <c r="AY6" s="0" t="n">
         <v>800</v>
       </c>
@@ -1725,9 +1711,6 @@
         <v>800</v>
       </c>
       <c r="BD6" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="BE6" s="0" t="n">
         <v>800</v>
       </c>
     </row>
@@ -1757,7 +1740,7 @@
         <v>800</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>800</v>
@@ -1781,7 +1764,7 @@
         <v>800</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="R7" s="0" t="n">
         <v>800</v>
@@ -1805,7 +1788,7 @@
         <v>800</v>
       </c>
       <c r="Y7" s="1" t="n">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="Z7" s="0" t="n">
         <v>800</v>
@@ -1828,10 +1811,10 @@
       <c r="AF7" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AG7" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AH7" s="1" t="n">
+      <c r="AG7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="0" t="n">
         <v>800</v>
       </c>
       <c r="AI7" s="0" t="n">
@@ -1852,11 +1835,11 @@
       <c r="AN7" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AO7" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AP7" s="2" t="n">
-        <v>0</v>
+      <c r="AO7" s="1" t="n">
+        <v>800</v>
+      </c>
+      <c r="AP7" s="0" t="n">
+        <v>800</v>
       </c>
       <c r="AQ7" s="0" t="n">
         <v>800</v>
@@ -1876,10 +1859,10 @@
       <c r="AV7" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="AW7" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="AX7" s="1" t="n">
+      <c r="AW7" s="1" t="n">
+        <v>800</v>
+      </c>
+      <c r="AX7" s="0" t="n">
         <v>800</v>
       </c>
       <c r="AY7" s="0" t="n">
@@ -1898,9 +1881,6 @@
         <v>800</v>
       </c>
       <c r="BD7" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="BE7" s="0" t="n">
         <v>800</v>
       </c>
     </row>
@@ -1930,7 +1910,7 @@
         <v>-200</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>-200</v>
+        <v>137</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>150</v>
@@ -1954,7 +1934,7 @@
         <v>-200</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <v>137</v>
+        <v>35</v>
       </c>
       <c r="R8" s="0" t="n">
         <v>-100</v>
@@ -1978,7 +1958,7 @@
         <v>-200</v>
       </c>
       <c r="Y8" s="1" t="n">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="Z8" s="0" t="n">
         <v>400</v>
@@ -2001,44 +1981,44 @@
       <c r="AF8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AG8" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="AH8" s="1" t="n">
-        <v>100</v>
+      <c r="AG8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="0" t="n">
+        <v>-300</v>
       </c>
       <c r="AI8" s="0" t="n">
         <v>-300</v>
       </c>
       <c r="AJ8" s="0" t="n">
-        <v>-300</v>
+        <v>-250</v>
       </c>
       <c r="AK8" s="0" t="n">
-        <v>-250</v>
+        <v>0</v>
       </c>
       <c r="AL8" s="0" t="n">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="AM8" s="0" t="n">
         <v>-100</v>
       </c>
       <c r="AN8" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="AO8" s="1" t="n">
         <v>-100</v>
       </c>
-      <c r="AO8" s="0" t="n">
+      <c r="AP8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="AR8" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="AP8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="0" t="n">
-        <v>400</v>
-      </c>
       <c r="AS8" s="0" t="n">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="AT8" s="0" t="n">
         <v>-100</v>
@@ -2047,33 +2027,30 @@
         <v>-100</v>
       </c>
       <c r="AV8" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="AW8" s="1" t="n">
+        <v>-200</v>
+      </c>
+      <c r="AX8" s="0" t="n">
+        <v>-200</v>
+      </c>
+      <c r="AY8" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="AW8" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="AX8" s="1" t="n">
-        <v>-100</v>
-      </c>
-      <c r="AY8" s="0" t="n">
+      <c r="AZ8" s="0" t="n">
         <v>-200</v>
-      </c>
-      <c r="AZ8" s="0" t="n">
-        <v>-100</v>
       </c>
       <c r="BA8" s="0" t="n">
         <v>-200</v>
       </c>
       <c r="BB8" s="0" t="n">
-        <v>-200</v>
+        <v>0</v>
       </c>
       <c r="BC8" s="0" t="n">
-        <v>0</v>
+        <v>-360</v>
       </c>
       <c r="BD8" s="0" t="n">
-        <v>-360</v>
-      </c>
-      <c r="BE8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2103,7 +2080,7 @@
         <v>500</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>0</v>
+        <v>182</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>420</v>
@@ -2127,7 +2104,7 @@
         <v>100</v>
       </c>
       <c r="Q9" s="1" t="n">
-        <v>182</v>
+        <v>-100</v>
       </c>
       <c r="R9" s="0" t="n">
         <v>100</v>
@@ -2151,7 +2128,7 @@
         <v>-300</v>
       </c>
       <c r="Y9" s="1" t="n">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="0" t="n">
         <v>100</v>
@@ -2174,79 +2151,76 @@
       <c r="AF9" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="AG9" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="AH9" s="1" t="n">
-        <v>0</v>
+      <c r="AG9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="0" t="n">
+        <v>100</v>
       </c>
       <c r="AI9" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="AJ9" s="0" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="AK9" s="0" t="n">
-        <v>0</v>
+        <v>-150</v>
       </c>
       <c r="AL9" s="0" t="n">
-        <v>-150</v>
+        <v>-100</v>
       </c>
       <c r="AM9" s="0" t="n">
         <v>-100</v>
       </c>
       <c r="AN9" s="0" t="n">
+        <v>-300</v>
+      </c>
+      <c r="AO9" s="1" t="n">
         <v>-100</v>
       </c>
-      <c r="AO9" s="0" t="n">
+      <c r="AP9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="AR9" s="0" t="n">
         <v>-300</v>
-      </c>
-      <c r="AP9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="0" t="n">
-        <v>100</v>
       </c>
       <c r="AS9" s="0" t="n">
         <v>-300</v>
       </c>
       <c r="AT9" s="0" t="n">
-        <v>-300</v>
+        <v>300</v>
       </c>
       <c r="AU9" s="0" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="AV9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AW9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="1" t="n">
-        <v>-100</v>
+      <c r="AW9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="0" t="n">
+        <v>200</v>
       </c>
       <c r="AY9" s="0" t="n">
         <v>200</v>
       </c>
       <c r="AZ9" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="BA9" s="0" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="BB9" s="0" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="BC9" s="0" t="n">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="BD9" s="0" t="n">
-        <v>-100</v>
-      </c>
-      <c r="BE9" s="0" t="n">
         <v>400</v>
       </c>
     </row>
@@ -2347,79 +2321,76 @@
       <c r="AF10" s="0" t="n">
         <v>-350</v>
       </c>
-      <c r="AG10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="1" t="n">
-        <v>0</v>
+      <c r="AG10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="0" t="n">
+        <v>-100</v>
       </c>
       <c r="AI10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="AJ10" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="AK10" s="0" t="n">
+        <v>-200</v>
+      </c>
+      <c r="AL10" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="AM10" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="AL10" s="0" t="n">
-        <v>-200</v>
-      </c>
-      <c r="AM10" s="0" t="n">
-        <v>140</v>
-      </c>
       <c r="AN10" s="0" t="n">
-        <v>-100</v>
-      </c>
-      <c r="AO10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ10" s="0" t="n">
-        <v>0</v>
+        <v>-360</v>
       </c>
       <c r="AR10" s="0" t="n">
-        <v>-360</v>
+        <v>100</v>
       </c>
       <c r="AS10" s="0" t="n">
         <v>100</v>
       </c>
       <c r="AT10" s="0" t="n">
-        <v>100</v>
+        <v>-200</v>
       </c>
       <c r="AU10" s="0" t="n">
+        <v>-300</v>
+      </c>
+      <c r="AV10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="0" t="n">
+        <v>-360</v>
+      </c>
+      <c r="AY10" s="0" t="n">
+        <v>-300</v>
+      </c>
+      <c r="AZ10" s="0" t="n">
         <v>-200</v>
       </c>
-      <c r="AV10" s="0" t="n">
-        <v>-300</v>
-      </c>
-      <c r="AW10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY10" s="0" t="n">
-        <v>-360</v>
-      </c>
-      <c r="AZ10" s="0" t="n">
-        <v>-300</v>
-      </c>
       <c r="BA10" s="0" t="n">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="BB10" s="0" t="n">
         <v>-100</v>
       </c>
       <c r="BC10" s="0" t="n">
-        <v>-100</v>
+        <v>-360</v>
       </c>
       <c r="BD10" s="0" t="n">
-        <v>-360</v>
-      </c>
-      <c r="BE10" s="0" t="n">
         <v>-200</v>
       </c>
     </row>
@@ -2520,11 +2491,11 @@
       <c r="AF11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AG11" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="AH11" s="1" t="n">
-        <v>0</v>
+      <c r="AG11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="0" t="n">
+        <v>-200</v>
       </c>
       <c r="AI11" s="0" t="n">
         <v>-200</v>
@@ -2536,63 +2507,60 @@
         <v>-200</v>
       </c>
       <c r="AL11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM11" s="0" t="n">
+        <v>-100</v>
+      </c>
+      <c r="AN11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="0" t="n">
         <v>-200</v>
       </c>
-      <c r="AM11" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="AN11" s="0" t="n">
+      <c r="AR11" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="AS11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="0" t="n">
+        <v>-200</v>
+      </c>
+      <c r="AU11" s="0" t="n">
+        <v>-350</v>
+      </c>
+      <c r="AV11" s="0" t="n">
+        <v>-200</v>
+      </c>
+      <c r="AW11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX11" s="0" t="n">
+        <v>-300</v>
+      </c>
+      <c r="AY11" s="0" t="n">
+        <v>-360</v>
+      </c>
+      <c r="AZ11" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="AO11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="0" t="n">
-        <v>-200</v>
-      </c>
-      <c r="AS11" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="AT11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="0" t="n">
-        <v>-200</v>
-      </c>
-      <c r="AV11" s="0" t="n">
-        <v>-350</v>
-      </c>
-      <c r="AW11" s="0" t="n">
-        <v>-200</v>
-      </c>
-      <c r="AX11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY11" s="0" t="n">
-        <v>-300</v>
-      </c>
-      <c r="AZ11" s="0" t="n">
+      <c r="BA11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB11" s="0" t="n">
         <v>-360</v>
       </c>
-      <c r="BA11" s="0" t="n">
+      <c r="BC11" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="BB11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC11" s="0" t="n">
-        <v>-360</v>
-      </c>
       <c r="BD11" s="0" t="n">
-        <v>-100</v>
-      </c>
-      <c r="BE11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2622,7 +2590,7 @@
         <v>500</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>0</v>
+        <v>187</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>600</v>
@@ -2646,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="n">
-        <v>187</v>
+        <v>-100</v>
       </c>
       <c r="R12" s="0" t="n">
         <v>200</v>
@@ -2670,7 +2638,7 @@
         <v>-300</v>
       </c>
       <c r="Y12" s="1" t="n">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="0" t="n">
         <v>200</v>
@@ -2693,65 +2661,65 @@
       <c r="AF12" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="AG12" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="AH12" s="1" t="n">
-        <v>0</v>
+      <c r="AG12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="0" t="n">
+        <v>100</v>
       </c>
       <c r="AI12" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AJ12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AK12" s="0" t="n">
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="AL12" s="0" t="n">
-        <v>-50</v>
+        <v>-100</v>
       </c>
       <c r="AM12" s="0" t="n">
         <v>-100</v>
       </c>
       <c r="AN12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO12" s="1" t="n">
         <v>-100</v>
       </c>
-      <c r="AO12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="2" t="n">
-        <v>0</v>
+      <c r="AP12" s="0" t="n">
+        <v>100</v>
       </c>
       <c r="AQ12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="0" t="n">
+        <v>-200</v>
+      </c>
+      <c r="AS12" s="0" t="n">
+        <v>-300</v>
+      </c>
+      <c r="AT12" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="AU12" s="0" t="n">
+        <v>-100</v>
+      </c>
+      <c r="AV12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX12" s="0" t="n">
         <v>100</v>
-      </c>
-      <c r="AR12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS12" s="0" t="n">
-        <v>-200</v>
-      </c>
-      <c r="AT12" s="0" t="n">
-        <v>-300</v>
-      </c>
-      <c r="AU12" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="AV12" s="0" t="n">
-        <v>-100</v>
-      </c>
-      <c r="AW12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX12" s="1" t="n">
-        <v>-100</v>
       </c>
       <c r="AY12" s="0" t="n">
         <v>100</v>
       </c>
       <c r="AZ12" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="BA12" s="0" t="n">
         <v>0</v>
@@ -2763,9 +2731,6 @@
         <v>0</v>
       </c>
       <c r="BD12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE12" s="0" t="n">
         <v>200</v>
       </c>
     </row>
@@ -2795,7 +2760,7 @@
         <v>200</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>200</v>
@@ -2819,7 +2784,7 @@
         <v>-200</v>
       </c>
       <c r="Q13" s="1" t="n">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="R13" s="0" t="n">
         <v>100</v>
@@ -2843,7 +2808,7 @@
         <v>-200</v>
       </c>
       <c r="Y13" s="1" t="n">
-        <v>118</v>
+        <v>50</v>
       </c>
       <c r="Z13" s="0" t="n">
         <v>-100</v>
@@ -2866,79 +2831,76 @@
       <c r="AF13" s="0" t="n">
         <v>-200</v>
       </c>
-      <c r="AG13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="1" t="n">
-        <v>50</v>
+      <c r="AG13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="AI13" s="0" t="n">
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="AJ13" s="0" t="n">
-        <v>-200</v>
+        <v>0</v>
       </c>
       <c r="AK13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AL13" s="0" t="n">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="AM13" s="0" t="n">
         <v>-100</v>
       </c>
       <c r="AN13" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="AO13" s="1" t="n">
         <v>-100</v>
       </c>
-      <c r="AO13" s="0" t="n">
+      <c r="AP13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="0" t="n">
+        <v>-100</v>
+      </c>
+      <c r="AR13" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="AS13" s="0" t="n">
+        <v>-300</v>
+      </c>
+      <c r="AT13" s="0" t="n">
+        <v>-100</v>
+      </c>
+      <c r="AU13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV13" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="AW13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX13" s="0" t="n">
+        <v>-150</v>
+      </c>
+      <c r="AY13" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="AP13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR13" s="0" t="n">
-        <v>-100</v>
-      </c>
-      <c r="AS13" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="AT13" s="0" t="n">
-        <v>-300</v>
-      </c>
-      <c r="AU13" s="0" t="n">
-        <v>-100</v>
-      </c>
-      <c r="AV13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW13" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="AX13" s="1" t="n">
-        <v>-100</v>
-      </c>
-      <c r="AY13" s="0" t="n">
-        <v>-150</v>
-      </c>
       <c r="AZ13" s="0" t="n">
-        <v>100</v>
+        <v>-200</v>
       </c>
       <c r="BA13" s="0" t="n">
-        <v>-200</v>
+        <v>0</v>
       </c>
       <c r="BB13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC13" s="0" t="n">
-        <v>0</v>
+        <v>-360</v>
       </c>
       <c r="BD13" s="0" t="n">
-        <v>-360</v>
-      </c>
-      <c r="BE13" s="0" t="n">
         <v>-200</v>
       </c>
     </row>
@@ -2992,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="R14" s="0" t="n">
         <v>0</v>
@@ -3016,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1" t="n">
-        <v>-50</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="0" t="n">
         <v>0</v>
@@ -3039,10 +3001,10 @@
       <c r="AF14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AG14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="1" t="n">
+      <c r="AG14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI14" s="0" t="n">
@@ -3063,10 +3025,10 @@
       <c r="AN14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AO14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP14" s="2" t="n">
+      <c r="AO14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ14" s="0" t="n">
@@ -3087,10 +3049,10 @@
       <c r="AV14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AW14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX14" s="1" t="n">
+      <c r="AW14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AY14" s="0" t="n">
@@ -3109,9 +3071,6 @@
         <v>0</v>
       </c>
       <c r="BD14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE14" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3165,7 +3124,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="R15" s="0" t="n">
         <v>0</v>
@@ -3189,7 +3148,7 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1" t="n">
-        <v>-50</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="0" t="n">
         <v>0</v>
@@ -3212,10 +3171,10 @@
       <c r="AF15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AG15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="1" t="n">
+      <c r="AG15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI15" s="0" t="n">
@@ -3236,10 +3195,10 @@
       <c r="AN15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AO15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP15" s="2" t="n">
+      <c r="AO15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ15" s="0" t="n">
@@ -3260,10 +3219,10 @@
       <c r="AV15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AW15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX15" s="1" t="n">
+      <c r="AW15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AY15" s="0" t="n">
@@ -3282,9 +3241,6 @@
         <v>0</v>
       </c>
       <c r="BD15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3385,10 +3341,10 @@
       <c r="AF16" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AG16" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AH16" s="1" t="n">
+      <c r="AG16" s="2" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AH16" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AI16" s="0" t="n">
@@ -3409,10 +3365,10 @@
       <c r="AN16" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AO16" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AP16" s="2" t="n">
+      <c r="AO16" s="1" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AP16" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AQ16" s="0" t="n">
@@ -3433,10 +3389,10 @@
       <c r="AV16" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AW16" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AX16" s="1" t="n">
+      <c r="AW16" s="1" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AX16" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AY16" s="0" t="n">
@@ -3455,9 +3411,6 @@
         <v>-1800</v>
       </c>
       <c r="BD16" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="BE16" s="0" t="n">
         <v>-1800</v>
       </c>
     </row>
@@ -3558,10 +3511,10 @@
       <c r="AF17" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AG17" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AH17" s="1" t="n">
+      <c r="AG17" s="2" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AH17" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AI17" s="0" t="n">
@@ -3582,10 +3535,10 @@
       <c r="AN17" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AO17" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AP17" s="2" t="n">
+      <c r="AO17" s="1" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AP17" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AQ17" s="0" t="n">
@@ -3606,10 +3559,10 @@
       <c r="AV17" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AW17" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AX17" s="1" t="n">
+      <c r="AW17" s="1" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AX17" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AY17" s="0" t="n">
@@ -3628,9 +3581,6 @@
         <v>-1800</v>
       </c>
       <c r="BD17" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="BE17" s="0" t="n">
         <v>-1800</v>
       </c>
     </row>
@@ -3731,10 +3681,10 @@
       <c r="AF18" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AG18" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AH18" s="1" t="n">
+      <c r="AG18" s="2" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AH18" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AI18" s="0" t="n">
@@ -3755,10 +3705,10 @@
       <c r="AN18" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AO18" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AP18" s="2" t="n">
+      <c r="AO18" s="1" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AP18" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AQ18" s="0" t="n">
@@ -3779,10 +3729,10 @@
       <c r="AV18" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AW18" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AX18" s="1" t="n">
+      <c r="AW18" s="1" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AX18" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AY18" s="0" t="n">
@@ -3801,9 +3751,6 @@
         <v>-1800</v>
       </c>
       <c r="BD18" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="BE18" s="0" t="n">
         <v>-1800</v>
       </c>
     </row>
@@ -3904,10 +3851,10 @@
       <c r="AF19" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AG19" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AH19" s="1" t="n">
+      <c r="AG19" s="2" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AH19" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AI19" s="0" t="n">
@@ -3928,10 +3875,10 @@
       <c r="AN19" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AO19" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AP19" s="2" t="n">
+      <c r="AO19" s="1" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AP19" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AQ19" s="0" t="n">
@@ -3952,10 +3899,10 @@
       <c r="AV19" s="0" t="n">
         <v>-1800</v>
       </c>
-      <c r="AW19" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="AX19" s="1" t="n">
+      <c r="AW19" s="1" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="AX19" s="0" t="n">
         <v>-1800</v>
       </c>
       <c r="AY19" s="0" t="n">
@@ -3974,9 +3921,6 @@
         <v>-1800</v>
       </c>
       <c r="BD19" s="0" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="BE19" s="0" t="n">
         <v>-1800</v>
       </c>
     </row>
@@ -4077,10 +4021,10 @@
       <c r="AF20" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AG20" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AH20" s="1" t="n">
+      <c r="AG20" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AH20" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AI20" s="0" t="n">
@@ -4101,10 +4045,10 @@
       <c r="AN20" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AO20" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AP20" s="2" t="n">
+      <c r="AO20" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AP20" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AQ20" s="0" t="n">
@@ -4125,10 +4069,10 @@
       <c r="AV20" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AW20" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AX20" s="1" t="n">
+      <c r="AW20" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AX20" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AY20" s="0" t="n">
@@ -4147,9 +4091,6 @@
         <v>1000</v>
       </c>
       <c r="BD20" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="BE20" s="0" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -4250,10 +4191,10 @@
       <c r="AF21" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AG21" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AH21" s="1" t="n">
+      <c r="AG21" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AH21" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AI21" s="0" t="n">
@@ -4274,10 +4215,10 @@
       <c r="AN21" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AO21" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AP21" s="2" t="n">
+      <c r="AO21" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AP21" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AQ21" s="0" t="n">
@@ -4298,10 +4239,10 @@
       <c r="AV21" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AW21" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AX21" s="1" t="n">
+      <c r="AW21" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AX21" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AY21" s="0" t="n">
@@ -4320,9 +4261,6 @@
         <v>1000</v>
       </c>
       <c r="BD21" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="BE21" s="0" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -4423,10 +4361,10 @@
       <c r="AF22" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AG22" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AH22" s="1" t="n">
+      <c r="AG22" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AH22" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AI22" s="0" t="n">
@@ -4447,10 +4385,10 @@
       <c r="AN22" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AO22" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AP22" s="2" t="n">
+      <c r="AO22" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AP22" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AQ22" s="0" t="n">
@@ -4471,10 +4409,10 @@
       <c r="AV22" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AW22" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AX22" s="1" t="n">
+      <c r="AW22" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AX22" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AY22" s="0" t="n">
@@ -4493,9 +4431,6 @@
         <v>1000</v>
       </c>
       <c r="BD22" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="BE22" s="0" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -4596,10 +4531,10 @@
       <c r="AF23" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AG23" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AH23" s="1" t="n">
+      <c r="AG23" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AH23" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AI23" s="0" t="n">
@@ -4620,10 +4555,10 @@
       <c r="AN23" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AO23" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AP23" s="2" t="n">
+      <c r="AO23" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AP23" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AQ23" s="0" t="n">
@@ -4644,10 +4579,10 @@
       <c r="AV23" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AW23" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="AX23" s="1" t="n">
+      <c r="AW23" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AX23" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AY23" s="0" t="n">
@@ -4666,9 +4601,6 @@
         <v>1000</v>
       </c>
       <c r="BD23" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="BE23" s="0" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -4698,7 +4630,7 @@
         <v>9143.44</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>10234.64</v>
+        <v>10770.32</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>7546.32</v>
@@ -4722,7 +4654,7 @@
         <v>4560.4</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>10770.32</v>
+        <v>11732.56</v>
       </c>
       <c r="R24" s="0" t="n">
         <v>7764.56</v>
@@ -4746,7 +4678,7 @@
         <v>6355.92</v>
       </c>
       <c r="Y24" s="1" t="n">
-        <v>11732.56</v>
+        <v>6524.56</v>
       </c>
       <c r="Z24" s="0" t="n">
         <v>3171.6</v>
@@ -4769,79 +4701,76 @@
       <c r="AF24" s="0" t="n">
         <v>6276.56</v>
       </c>
-      <c r="AG24" s="0" t="n">
-        <v>10968.72</v>
-      </c>
-      <c r="AH24" s="1" t="n">
-        <v>6524.56</v>
+      <c r="AG24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="0" t="n">
+        <v>6484.88</v>
       </c>
       <c r="AI24" s="0" t="n">
-        <v>6484.88</v>
+        <v>7209.04</v>
       </c>
       <c r="AJ24" s="0" t="n">
-        <v>7209.04</v>
+        <v>13131.28</v>
       </c>
       <c r="AK24" s="0" t="n">
-        <v>13131.28</v>
+        <v>5205.2</v>
       </c>
       <c r="AL24" s="0" t="n">
-        <v>5205.2</v>
+        <v>4362</v>
       </c>
       <c r="AM24" s="0" t="n">
-        <v>4362</v>
+        <v>3667.6</v>
       </c>
       <c r="AN24" s="0" t="n">
-        <v>3667.6</v>
-      </c>
-      <c r="AO24" s="0" t="n">
         <v>2735.12</v>
       </c>
-      <c r="AP24" s="2" t="n">
-        <v>0</v>
+      <c r="AO24" s="1" t="n">
+        <v>11871.44</v>
+      </c>
+      <c r="AP24" s="0" t="n">
+        <v>8518.48</v>
       </c>
       <c r="AQ24" s="0" t="n">
-        <v>8518.48</v>
+        <v>2219.28</v>
       </c>
       <c r="AR24" s="0" t="n">
-        <v>2219.28</v>
+        <v>2318.48</v>
       </c>
       <c r="AS24" s="0" t="n">
-        <v>2318.48</v>
+        <v>5195.28</v>
       </c>
       <c r="AT24" s="0" t="n">
-        <v>5195.28</v>
+        <v>4490.96</v>
       </c>
       <c r="AU24" s="0" t="n">
-        <v>4490.96</v>
+        <v>5453.2</v>
       </c>
       <c r="AV24" s="0" t="n">
-        <v>5453.2</v>
-      </c>
-      <c r="AW24" s="0" t="n">
         <v>542.8</v>
       </c>
-      <c r="AX24" s="1" t="n">
-        <v>11871.44</v>
+      <c r="AW24" s="1" t="n">
+        <v>10234.64</v>
+      </c>
+      <c r="AX24" s="0" t="n">
+        <v>2854.16</v>
       </c>
       <c r="AY24" s="0" t="n">
+        <v>3082.32</v>
+      </c>
+      <c r="AZ24" s="0" t="n">
         <v>2854.16</v>
       </c>
-      <c r="AZ24" s="0" t="n">
-        <v>3082.32</v>
-      </c>
       <c r="BA24" s="0" t="n">
-        <v>2854.16</v>
+        <v>9827.92</v>
       </c>
       <c r="BB24" s="0" t="n">
-        <v>9827.92</v>
+        <v>4590.16</v>
       </c>
       <c r="BC24" s="0" t="n">
-        <v>4590.16</v>
+        <v>8865.68</v>
       </c>
       <c r="BD24" s="0" t="n">
-        <v>8865.68</v>
-      </c>
-      <c r="BE24" s="0" t="n">
         <v>3885.84</v>
       </c>
     </row>
@@ -4871,7 +4800,7 @@
         <v>3052.56</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>17942.48</v>
+        <v>16950.48</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>6088.08</v>
@@ -4895,7 +4824,7 @@
         <v>6822.16</v>
       </c>
       <c r="Q25" s="1" t="n">
-        <v>16950.48</v>
+        <v>21979.92</v>
       </c>
       <c r="R25" s="0" t="n">
         <v>4719.12</v>
@@ -4919,7 +4848,7 @@
         <v>6792.4</v>
       </c>
       <c r="Y25" s="1" t="n">
-        <v>21979.92</v>
+        <v>19351.12</v>
       </c>
       <c r="Z25" s="0" t="n">
         <v>4262.8</v>
@@ -4942,79 +4871,76 @@
       <c r="AF25" s="0" t="n">
         <v>3231.12</v>
       </c>
-      <c r="AG25" s="0" t="n">
-        <v>10869.52</v>
-      </c>
-      <c r="AH25" s="1" t="n">
-        <v>19351.12</v>
+      <c r="AG25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="0" t="n">
+        <v>4451.28</v>
       </c>
       <c r="AI25" s="0" t="n">
+        <v>4758.8</v>
+      </c>
+      <c r="AJ25" s="0" t="n">
+        <v>6078.16</v>
+      </c>
+      <c r="AK25" s="0" t="n">
+        <v>1336.4</v>
+      </c>
+      <c r="AL25" s="0" t="n">
+        <v>6673.36</v>
+      </c>
+      <c r="AM25" s="0" t="n">
+        <v>4639.76</v>
+      </c>
+      <c r="AN25" s="0" t="n">
+        <v>7962.96</v>
+      </c>
+      <c r="AO25" s="1" t="n">
+        <v>8706.96</v>
+      </c>
+      <c r="AP25" s="0" t="n">
+        <v>4967.12</v>
+      </c>
+      <c r="AQ25" s="0" t="n">
+        <v>3657.68</v>
+      </c>
+      <c r="AR25" s="0" t="n">
+        <v>6286.48</v>
+      </c>
+      <c r="AS25" s="0" t="n">
+        <v>6117.84</v>
+      </c>
+      <c r="AT25" s="0" t="n">
+        <v>6752.72</v>
+      </c>
+      <c r="AU25" s="0" t="n">
+        <v>6395.6</v>
+      </c>
+      <c r="AV25" s="0" t="n">
+        <v>7159.44</v>
+      </c>
+      <c r="AW25" s="1" t="n">
+        <v>17942.48</v>
+      </c>
+      <c r="AX25" s="0" t="n">
+        <v>6673.36</v>
+      </c>
+      <c r="AY25" s="0" t="n">
+        <v>5701.2</v>
+      </c>
+      <c r="AZ25" s="0" t="n">
+        <v>4282.64</v>
+      </c>
+      <c r="BA25" s="0" t="n">
+        <v>2020.88</v>
+      </c>
+      <c r="BB25" s="0" t="n">
+        <v>6613.84</v>
+      </c>
+      <c r="BC25" s="0" t="n">
         <v>4451.28</v>
       </c>
-      <c r="AJ25" s="0" t="n">
-        <v>4758.8</v>
-      </c>
-      <c r="AK25" s="0" t="n">
-        <v>6078.16</v>
-      </c>
-      <c r="AL25" s="0" t="n">
-        <v>1336.4</v>
-      </c>
-      <c r="AM25" s="0" t="n">
-        <v>6673.36</v>
-      </c>
-      <c r="AN25" s="0" t="n">
-        <v>4639.76</v>
-      </c>
-      <c r="AO25" s="0" t="n">
-        <v>7962.96</v>
-      </c>
-      <c r="AP25" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ25" s="0" t="n">
-        <v>4967.12</v>
-      </c>
-      <c r="AR25" s="0" t="n">
-        <v>3657.68</v>
-      </c>
-      <c r="AS25" s="0" t="n">
-        <v>6286.48</v>
-      </c>
-      <c r="AT25" s="0" t="n">
-        <v>6117.84</v>
-      </c>
-      <c r="AU25" s="0" t="n">
-        <v>6752.72</v>
-      </c>
-      <c r="AV25" s="0" t="n">
-        <v>6395.6</v>
-      </c>
-      <c r="AW25" s="0" t="n">
-        <v>7159.44</v>
-      </c>
-      <c r="AX25" s="1" t="n">
-        <v>8706.96</v>
-      </c>
-      <c r="AY25" s="0" t="n">
-        <v>6673.36</v>
-      </c>
-      <c r="AZ25" s="0" t="n">
-        <v>5701.2</v>
-      </c>
-      <c r="BA25" s="0" t="n">
-        <v>4282.64</v>
-      </c>
-      <c r="BB25" s="0" t="n">
-        <v>2020.88</v>
-      </c>
-      <c r="BC25" s="0" t="n">
-        <v>6613.84</v>
-      </c>
       <c r="BD25" s="0" t="n">
-        <v>4451.28</v>
-      </c>
-      <c r="BE25" s="0" t="n">
         <v>2814.48</v>
       </c>
     </row>
@@ -5044,7 +4970,7 @@
         <v>14272.08</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>-230.96</v>
+        <v>7.12</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>8597.84</v>
@@ -5068,7 +4994,7 @@
         <v>5621.84</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <v>7.12</v>
+        <v>-82.16</v>
       </c>
       <c r="R26" s="0" t="n">
         <v>4689.36</v>
@@ -5092,7 +5018,7 @@
         <v>6306.32</v>
       </c>
       <c r="Y26" s="1" t="n">
-        <v>-82.16</v>
+        <v>0</v>
       </c>
       <c r="Z26" s="0" t="n">
         <v>5175.44</v>
@@ -5115,79 +5041,76 @@
       <c r="AF26" s="0" t="n">
         <v>8597.84</v>
       </c>
-      <c r="AG26" s="0" t="n">
-        <v>9371.6</v>
-      </c>
-      <c r="AH26" s="1" t="n">
-        <v>0</v>
+      <c r="AG26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="0" t="n">
+        <v>5443.28</v>
       </c>
       <c r="AI26" s="0" t="n">
-        <v>5443.28</v>
+        <v>6236.88</v>
       </c>
       <c r="AJ26" s="0" t="n">
-        <v>6236.88</v>
+        <v>6742.8</v>
       </c>
       <c r="AK26" s="0" t="n">
-        <v>6742.8</v>
+        <v>3022.8</v>
       </c>
       <c r="AL26" s="0" t="n">
-        <v>3022.8</v>
+        <v>4550.48</v>
       </c>
       <c r="AM26" s="0" t="n">
-        <v>4550.48</v>
+        <v>3568.4</v>
       </c>
       <c r="AN26" s="0" t="n">
+        <v>5244.88</v>
+      </c>
+      <c r="AO26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP26" s="0" t="n">
+        <v>8954.96</v>
+      </c>
+      <c r="AQ26" s="0" t="n">
+        <v>8607.76</v>
+      </c>
+      <c r="AR26" s="0" t="n">
         <v>3568.4</v>
       </c>
-      <c r="AO26" s="0" t="n">
-        <v>5244.88</v>
-      </c>
-      <c r="AP26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ26" s="0" t="n">
-        <v>8954.96</v>
-      </c>
-      <c r="AR26" s="0" t="n">
-        <v>8607.76</v>
-      </c>
       <c r="AS26" s="0" t="n">
-        <v>3568.4</v>
+        <v>3399.76</v>
       </c>
       <c r="AT26" s="0" t="n">
-        <v>3399.76</v>
+        <v>6752.72</v>
       </c>
       <c r="AU26" s="0" t="n">
-        <v>6752.72</v>
+        <v>6008.72</v>
       </c>
       <c r="AV26" s="0" t="n">
-        <v>6008.72</v>
-      </c>
-      <c r="AW26" s="0" t="n">
         <v>4233.04</v>
       </c>
-      <c r="AX26" s="1" t="n">
-        <v>0</v>
+      <c r="AW26" s="1" t="n">
+        <v>-230.96</v>
+      </c>
+      <c r="AX26" s="0" t="n">
+        <v>7020.56</v>
       </c>
       <c r="AY26" s="0" t="n">
-        <v>7020.56</v>
+        <v>4610</v>
       </c>
       <c r="AZ26" s="0" t="n">
-        <v>4610</v>
+        <v>3459.28</v>
       </c>
       <c r="BA26" s="0" t="n">
-        <v>3459.28</v>
+        <v>9956.88</v>
       </c>
       <c r="BB26" s="0" t="n">
-        <v>9956.88</v>
+        <v>5602</v>
       </c>
       <c r="BC26" s="0" t="n">
-        <v>5602</v>
+        <v>7714.96</v>
       </c>
       <c r="BD26" s="0" t="n">
-        <v>7714.96</v>
-      </c>
-      <c r="BE26" s="0" t="n">
         <v>5750.8</v>
       </c>
     </row>
@@ -5217,7 +5140,7 @@
         <v>10234.64</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>-230.96</v>
+        <v>-12.72</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>11008.4</v>
@@ -5241,7 +5164,7 @@
         <v>4818.32</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <v>-12.72</v>
+        <v>-111.92</v>
       </c>
       <c r="R27" s="0" t="n">
         <v>6663.44</v>
@@ -5265,7 +5188,7 @@
         <v>4362</v>
       </c>
       <c r="Y27" s="1" t="n">
-        <v>-111.92</v>
+        <v>0</v>
       </c>
       <c r="Z27" s="0" t="n">
         <v>4858</v>
@@ -5288,79 +5211,76 @@
       <c r="AF27" s="0" t="n">
         <v>4937.36</v>
       </c>
-      <c r="AG27" s="0" t="n">
-        <v>11613.52</v>
-      </c>
-      <c r="AH27" s="1" t="n">
-        <v>0</v>
+      <c r="AG27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="0" t="n">
+        <v>3151.76</v>
       </c>
       <c r="AI27" s="0" t="n">
-        <v>3151.76</v>
+        <v>4114</v>
       </c>
       <c r="AJ27" s="0" t="n">
-        <v>4114</v>
+        <v>10780.24</v>
       </c>
       <c r="AK27" s="0" t="n">
-        <v>10780.24</v>
+        <v>2298.64</v>
       </c>
       <c r="AL27" s="0" t="n">
-        <v>2298.64</v>
+        <v>7020.56</v>
       </c>
       <c r="AM27" s="0" t="n">
-        <v>7020.56</v>
+        <v>2874</v>
       </c>
       <c r="AN27" s="0" t="n">
-        <v>2874</v>
-      </c>
-      <c r="AO27" s="0" t="n">
         <v>4570.32</v>
       </c>
-      <c r="AP27" s="2" t="n">
-        <v>0</v>
+      <c r="AO27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP27" s="0" t="n">
+        <v>9510.48</v>
       </c>
       <c r="AQ27" s="0" t="n">
-        <v>9510.48</v>
+        <v>3379.92</v>
       </c>
       <c r="AR27" s="0" t="n">
-        <v>3379.92</v>
+        <v>5443.28</v>
       </c>
       <c r="AS27" s="0" t="n">
-        <v>5443.28</v>
+        <v>3181.52</v>
       </c>
       <c r="AT27" s="0" t="n">
-        <v>3181.52</v>
+        <v>3707.28</v>
       </c>
       <c r="AU27" s="0" t="n">
-        <v>3707.28</v>
+        <v>9202.96</v>
       </c>
       <c r="AV27" s="0" t="n">
-        <v>9202.96</v>
-      </c>
-      <c r="AW27" s="0" t="n">
         <v>6256.72</v>
       </c>
-      <c r="AX27" s="1" t="n">
-        <v>0</v>
+      <c r="AW27" s="1" t="n">
+        <v>-230.96</v>
+      </c>
+      <c r="AX27" s="0" t="n">
+        <v>3360.08</v>
       </c>
       <c r="AY27" s="0" t="n">
-        <v>3360.08</v>
+        <v>9589.84</v>
       </c>
       <c r="AZ27" s="0" t="n">
-        <v>9589.84</v>
+        <v>6107.92</v>
       </c>
       <c r="BA27" s="0" t="n">
-        <v>6107.92</v>
+        <v>6395.6</v>
       </c>
       <c r="BB27" s="0" t="n">
-        <v>6395.6</v>
+        <v>7457.04</v>
       </c>
       <c r="BC27" s="0" t="n">
-        <v>7457.04</v>
+        <v>1842.32</v>
       </c>
       <c r="BD27" s="0" t="n">
-        <v>1842.32</v>
-      </c>
-      <c r="BE27" s="0" t="n">
         <v>2001.04</v>
       </c>
     </row>
@@ -5390,7 +5310,7 @@
         <v>1733.2</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>17565.52</v>
+        <v>16216.4</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>4193.36</v>
@@ -5414,7 +5334,7 @@
         <v>6643.6</v>
       </c>
       <c r="Q28" s="1" t="n">
-        <v>16216.4</v>
+        <v>23596.88</v>
       </c>
       <c r="R28" s="0" t="n">
         <v>4173.52</v>
@@ -5438,7 +5358,7 @@
         <v>6197.2</v>
       </c>
       <c r="Y28" s="1" t="n">
-        <v>23596.88</v>
+        <v>17972.24</v>
       </c>
       <c r="Z28" s="0" t="n">
         <v>2943.44</v>
@@ -5461,79 +5381,76 @@
       <c r="AF28" s="0" t="n">
         <v>4342.16</v>
       </c>
-      <c r="AG28" s="0" t="n">
-        <v>9689.04</v>
-      </c>
-      <c r="AH28" s="1" t="n">
-        <v>17972.24</v>
+      <c r="AG28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="0" t="n">
+        <v>5443.28</v>
       </c>
       <c r="AI28" s="0" t="n">
-        <v>5443.28</v>
+        <v>5344.08</v>
       </c>
       <c r="AJ28" s="0" t="n">
-        <v>5344.08</v>
+        <v>5760.72</v>
       </c>
       <c r="AK28" s="0" t="n">
-        <v>5760.72</v>
+        <v>2050.64</v>
       </c>
       <c r="AL28" s="0" t="n">
-        <v>2050.64</v>
+        <v>5721.04</v>
       </c>
       <c r="AM28" s="0" t="n">
-        <v>5721.04</v>
+        <v>6703.12</v>
       </c>
       <c r="AN28" s="0" t="n">
-        <v>6703.12</v>
-      </c>
-      <c r="AO28" s="0" t="n">
         <v>6395.6</v>
       </c>
-      <c r="AP28" s="2" t="n">
-        <v>0</v>
+      <c r="AO28" s="1" t="n">
+        <v>14440.72</v>
+      </c>
+      <c r="AP28" s="0" t="n">
+        <v>4709.2</v>
       </c>
       <c r="AQ28" s="0" t="n">
-        <v>4709.2</v>
+        <v>6107.92</v>
       </c>
       <c r="AR28" s="0" t="n">
-        <v>6107.92</v>
+        <v>4530.64</v>
       </c>
       <c r="AS28" s="0" t="n">
-        <v>4530.64</v>
+        <v>9262.48</v>
       </c>
       <c r="AT28" s="0" t="n">
-        <v>9262.48</v>
+        <v>3657.68</v>
       </c>
       <c r="AU28" s="0" t="n">
-        <v>3657.68</v>
+        <v>7506.64</v>
       </c>
       <c r="AV28" s="0" t="n">
-        <v>7506.64</v>
-      </c>
-      <c r="AW28" s="0" t="n">
         <v>5899.6</v>
       </c>
-      <c r="AX28" s="1" t="n">
-        <v>14440.72</v>
+      <c r="AW28" s="1" t="n">
+        <v>17565.52</v>
+      </c>
+      <c r="AX28" s="0" t="n">
+        <v>5830.16</v>
       </c>
       <c r="AY28" s="0" t="n">
-        <v>5830.16</v>
+        <v>5542.48</v>
       </c>
       <c r="AZ28" s="0" t="n">
-        <v>5542.48</v>
+        <v>6445.2</v>
       </c>
       <c r="BA28" s="0" t="n">
-        <v>6445.2</v>
+        <v>2556.56</v>
       </c>
       <c r="BB28" s="0" t="n">
-        <v>2556.56</v>
+        <v>6425.36</v>
       </c>
       <c r="BC28" s="0" t="n">
-        <v>6425.36</v>
+        <v>4748.88</v>
       </c>
       <c r="BD28" s="0" t="n">
-        <v>4748.88</v>
-      </c>
-      <c r="BE28" s="0" t="n">
         <v>2963.28</v>
       </c>
     </row>
@@ -5563,7 +5480,7 @@
         <v>7288.4</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>6365.84</v>
+        <v>9282.32</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>5939.28</v>
@@ -5587,7 +5504,7 @@
         <v>4500.88</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>9282.32</v>
+        <v>8181.2</v>
       </c>
       <c r="R29" s="0" t="n">
         <v>4977.04</v>
@@ -5611,7 +5528,7 @@
         <v>6484.88</v>
       </c>
       <c r="Y29" s="1" t="n">
-        <v>8181.2</v>
+        <v>13379.28</v>
       </c>
       <c r="Z29" s="0" t="n">
         <v>2536.72</v>
@@ -5634,79 +5551,76 @@
       <c r="AF29" s="0" t="n">
         <v>3250.96</v>
       </c>
-      <c r="AG29" s="0" t="n">
-        <v>10135.44</v>
-      </c>
-      <c r="AH29" s="1" t="n">
-        <v>13379.28</v>
+      <c r="AG29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH29" s="0" t="n">
+        <v>3389.84</v>
       </c>
       <c r="AI29" s="0" t="n">
-        <v>3389.84</v>
+        <v>7030.48</v>
       </c>
       <c r="AJ29" s="0" t="n">
-        <v>7030.48</v>
+        <v>3350.16</v>
       </c>
       <c r="AK29" s="0" t="n">
-        <v>3350.16</v>
+        <v>7843.92</v>
       </c>
       <c r="AL29" s="0" t="n">
-        <v>7843.92</v>
+        <v>4441.36</v>
       </c>
       <c r="AM29" s="0" t="n">
-        <v>4441.36</v>
+        <v>3370</v>
       </c>
       <c r="AN29" s="0" t="n">
-        <v>3370</v>
-      </c>
-      <c r="AO29" s="0" t="n">
         <v>4431.44</v>
       </c>
-      <c r="AP29" s="2" t="n">
-        <v>0</v>
+      <c r="AO29" s="1" t="n">
+        <v>5175.44</v>
+      </c>
+      <c r="AP29" s="0" t="n">
+        <v>7764.56</v>
       </c>
       <c r="AQ29" s="0" t="n">
-        <v>7764.56</v>
+        <v>1941.52</v>
       </c>
       <c r="AR29" s="0" t="n">
-        <v>1941.52</v>
+        <v>3727.12</v>
       </c>
       <c r="AS29" s="0" t="n">
-        <v>3727.12</v>
+        <v>9450.96</v>
       </c>
       <c r="AT29" s="0" t="n">
-        <v>9450.96</v>
+        <v>3796.56</v>
       </c>
       <c r="AU29" s="0" t="n">
-        <v>3796.56</v>
+        <v>5155.6</v>
       </c>
       <c r="AV29" s="0" t="n">
-        <v>5155.6</v>
-      </c>
-      <c r="AW29" s="0" t="n">
         <v>3270.8</v>
       </c>
-      <c r="AX29" s="1" t="n">
-        <v>5175.44</v>
+      <c r="AW29" s="1" t="n">
+        <v>6365.84</v>
+      </c>
+      <c r="AX29" s="0" t="n">
+        <v>4024.72</v>
       </c>
       <c r="AY29" s="0" t="n">
-        <v>4024.72</v>
+        <v>5641.68</v>
       </c>
       <c r="AZ29" s="0" t="n">
-        <v>5641.68</v>
+        <v>3856.08</v>
       </c>
       <c r="BA29" s="0" t="n">
-        <v>3856.08</v>
+        <v>4877.84</v>
       </c>
       <c r="BB29" s="0" t="n">
-        <v>4877.84</v>
+        <v>5651.6</v>
       </c>
       <c r="BC29" s="0" t="n">
-        <v>5651.6</v>
+        <v>4977.04</v>
       </c>
       <c r="BD29" s="0" t="n">
-        <v>4977.04</v>
-      </c>
-      <c r="BE29" s="0" t="n">
         <v>4114</v>
       </c>
     </row>
@@ -5726,17 +5640,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D67" activeCellId="0" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6012,214 +5926,210 @@
         <v>121</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>123</v>
+      </c>
       <c r="B34" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>131</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>140</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B57" s="0" t="s">
         <v>55</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rename STRIP08 to STRIP8 to make the webserver happy
</commit_message>
<xml_diff>
--- a/data/default_biases_warm.xlsx
+++ b/data/default_biases_warm.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
   <si>
     <t>PAR</t>
   </si>
@@ -370,9 +370,6 @@
   </si>
   <si>
     <t>Y3</t>
-  </si>
-  <si>
-    <t>STRIP08</t>
   </si>
   <si>
     <t>Y4</t>
@@ -470,8 +467,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -502,9 +499,19 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -516,10 +523,45 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -530,11 +572,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -553,21 +595,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -576,24 +603,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -606,38 +632,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -651,10 +647,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -673,7 +670,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,19 +694,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,7 +712,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -721,25 +802,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,109 +838,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -901,15 +898,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -920,6 +908,30 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -949,157 +961,142 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6451,8 +6448,8 @@
   <sheetPr/>
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="2"/>
@@ -6703,12 +6700,12 @@
         <v>117</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -6716,7 +6713,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -6724,7 +6721,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
         <v>27</v>
@@ -6732,18 +6729,18 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s">
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" t="s">
         <v>38</v>
@@ -6751,7 +6748,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" t="s">
         <v>39</v>
@@ -6759,7 +6756,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
@@ -6767,7 +6764,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -6775,7 +6772,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
@@ -6783,7 +6780,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -6791,7 +6788,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B40" t="s">
         <v>33</v>
@@ -6799,18 +6796,18 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B41" t="s">
         <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
@@ -6818,7 +6815,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" t="s">
         <v>46</v>
@@ -6826,7 +6823,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B44" t="s">
         <v>41</v>
@@ -6834,7 +6831,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B45" t="s">
         <v>47</v>
@@ -6842,7 +6839,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B46" t="s">
         <v>44</v>
@@ -6850,7 +6847,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B47" t="s">
         <v>48</v>
@@ -6858,7 +6855,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B48" t="s">
         <v>42</v>
@@ -6866,18 +6863,18 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B49" t="s">
         <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s">
         <v>51</v>
@@ -6885,7 +6882,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
         <v>52</v>
@@ -6893,7 +6890,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B52" t="s">
         <v>49</v>
@@ -6901,7 +6898,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B53" t="s">
         <v>53</v>
@@ -6909,7 +6906,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
         <v>50</v>
@@ -6917,7 +6914,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B55" t="s">
         <v>55</v>
@@ -6925,7 +6922,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Fix entry for STRIP08 (Y3)
</commit_message>
<xml_diff>
--- a/data/default_biases_warm.xlsx
+++ b/data/default_biases_warm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12420" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Biases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="149">
   <si>
     <t>PAR</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>Y3</t>
+  </si>
+  <si>
+    <t>STRIP08</t>
   </si>
   <si>
     <t>Y4</t>
@@ -467,10 +470,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -499,12 +502,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -514,37 +514,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -559,37 +530,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -603,8 +552,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -626,13 +607,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -641,15 +615,44 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -676,13 +679,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -694,19 +691,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -724,31 +721,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -760,31 +751,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,25 +769,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,13 +787,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,7 +805,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -879,21 +882,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -905,18 +893,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -951,160 +932,182 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1353,7 +1356,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1377,9 +1380,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1403,7 +1406,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1456,7 +1459,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1481,7 +1484,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1501,9 +1504,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1022" width="8.55333333333333" customWidth="1"/>
+    <col min="1" max="1022" width="8.55333333333333" customWidth="true"/>
     <col min="1023" max="1023" width="11.52"/>
-    <col min="1024" max="1025" width="9.14" customWidth="1"/>
+    <col min="1024" max="1025" width="9.14" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56">
@@ -6438,7 +6441,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -6454,9 +6457,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="7.82666666666667" customWidth="1"/>
-    <col min="2" max="2" width="11.1066666666667" customWidth="1"/>
-    <col min="3" max="1025" width="8.55333333333333" customWidth="1"/>
+    <col min="1" max="1" width="7.82666666666667" customWidth="true"/>
+    <col min="2" max="2" width="11.1066666666667" customWidth="true"/>
+    <col min="3" max="1025" width="8.55333333333333" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6700,12 +6703,12 @@
         <v>117</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -6713,7 +6716,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -6721,7 +6724,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B32" t="s">
         <v>27</v>
@@ -6729,18 +6732,18 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
         <v>38</v>
@@ -6748,7 +6751,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B35" t="s">
         <v>39</v>
@@ -6756,7 +6759,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
@@ -6764,7 +6767,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -6772,7 +6775,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
@@ -6780,7 +6783,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -6788,7 +6791,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B40" t="s">
         <v>33</v>
@@ -6796,18 +6799,18 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s">
         <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
@@ -6815,7 +6818,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B43" t="s">
         <v>46</v>
@@ -6823,7 +6826,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B44" t="s">
         <v>41</v>
@@ -6831,7 +6834,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B45" t="s">
         <v>47</v>
@@ -6839,7 +6842,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B46" t="s">
         <v>44</v>
@@ -6847,7 +6850,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s">
         <v>48</v>
@@ -6855,7 +6858,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B48" t="s">
         <v>42</v>
@@ -6863,18 +6866,18 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B49" t="s">
         <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
         <v>51</v>
@@ -6882,7 +6885,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B51" t="s">
         <v>52</v>
@@ -6890,7 +6893,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B52" t="s">
         <v>49</v>
@@ -6898,7 +6901,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
         <v>53</v>
@@ -6906,7 +6909,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
         <v>50</v>
@@ -6914,7 +6917,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B55" t="s">
         <v>55</v>
@@ -6922,7 +6925,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
@@ -6930,7 +6933,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Fix warm bias table
</commit_message>
<xml_diff>
--- a/data/default_biases_warm.xlsx
+++ b/data/default_biases_warm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Biases" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
   <si>
     <t xml:space="preserve">PAR</t>
   </si>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">STRIP73</t>
   </si>
   <si>
-    <t xml:space="preserve">STRIP8</t>
+    <t xml:space="preserve">STRIP08</t>
   </si>
   <si>
     <t xml:space="preserve">STRIP48</t>
@@ -366,9 +366,6 @@
   </si>
   <si>
     <t xml:space="preserve">Y0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRIP08</t>
   </si>
   <si>
     <t xml:space="preserve">Y1</t>
@@ -686,8 +683,8 @@
   </sheetPr>
   <dimension ref="A1:BD29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW1" activeCellId="0" sqref="AW1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z2" activeCellId="0" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5644,8 +5641,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5871,12 +5868,12 @@
         <v>114</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>115</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>26</v>
@@ -5884,7 +5881,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>27</v>
@@ -5892,7 +5889,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>28</v>
@@ -5900,7 +5897,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>29</v>
@@ -5908,7 +5905,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>30</v>
@@ -5916,7 +5913,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>31</v>
@@ -5924,18 +5921,18 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>33</v>
@@ -5943,7 +5940,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>34</v>
@@ -5951,7 +5948,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>35</v>
@@ -5959,7 +5956,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>36</v>
@@ -5967,7 +5964,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>37</v>
@@ -5975,7 +5972,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>38</v>
@@ -5983,7 +5980,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>39</v>
@@ -5991,18 +5988,18 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>41</v>
@@ -6010,7 +6007,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>42</v>
@@ -6018,7 +6015,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>43</v>
@@ -6026,7 +6023,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>44</v>
@@ -6034,7 +6031,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>45</v>
@@ -6042,7 +6039,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>46</v>
@@ -6050,7 +6047,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>47</v>
@@ -6058,18 +6055,18 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>49</v>
@@ -6077,7 +6074,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>50</v>
@@ -6085,7 +6082,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>51</v>
@@ -6093,7 +6090,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>52</v>
@@ -6101,7 +6098,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>53</v>
@@ -6109,7 +6106,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>54</v>
@@ -6117,7 +6114,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Move from Travis to GitHub Actions (#48)
</commit_message>
<xml_diff>
--- a/data/default_biases_warm.xlsx
+++ b/data/default_biases_warm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Biases" sheetId="1" state="visible" r:id="rId2"/>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">STRIP73</t>
   </si>
   <si>
-    <t xml:space="preserve">STRIP08</t>
+    <t xml:space="preserve">STRIP8</t>
   </si>
   <si>
     <t xml:space="preserve">STRIP48</t>
@@ -677,20 +677,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:BD29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z2" activeCellId="0" sqref="Z2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AW1" activeCellId="0" sqref="AW1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1" style="0" width="8.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5625,8 +5626,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5635,20 +5636,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D67" activeCellId="0" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6124,10 +6126,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add detectors hks to bias tables (warm/cryo)
</commit_message>
<xml_diff>
--- a/data/default_biases_warm.xlsx
+++ b/data/default_biases_warm.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="160">
   <si>
     <t>PAR</t>
   </si>
@@ -273,6 +273,42 @@
   </si>
   <si>
     <t>ID5</t>
+  </si>
+  <si>
+    <t>DET0_BIAS</t>
+  </si>
+  <si>
+    <t>DET1_BIAS</t>
+  </si>
+  <si>
+    <t>DET2_BIAS</t>
+  </si>
+  <si>
+    <t>DET3_BIAS</t>
+  </si>
+  <si>
+    <t>DET0_OFFSET</t>
+  </si>
+  <si>
+    <t>DET1_OFFSET</t>
+  </si>
+  <si>
+    <t>DET2_OFFSET</t>
+  </si>
+  <si>
+    <t>DET3_OFFSET</t>
+  </si>
+  <si>
+    <t>DET0_GAIN</t>
+  </si>
+  <si>
+    <t>DET1_GAIN</t>
+  </si>
+  <si>
+    <t>DET2_GAIN</t>
+  </si>
+  <si>
+    <t>DET3_GAIN</t>
   </si>
   <si>
     <t>Module</t>
@@ -473,9 +509,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -511,9 +547,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -527,8 +562,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -541,19 +577,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -572,10 +608,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -587,21 +624,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -610,16 +632,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -634,22 +655,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -664,13 +700,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,102 +736,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -796,7 +748,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,19 +856,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,7 +868,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,7 +880,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -873,15 +909,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -893,6 +920,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -912,11 +948,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -931,177 +991,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1432,15 +1468,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BD29"/>
+  <dimension ref="A1:BD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AV7" sqref="AV7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1021" width="8.5462962962963" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8888888888889" style="1" customWidth="1"/>
+    <col min="2" max="1021" width="8.5462962962963" style="1" customWidth="1"/>
     <col min="1022" max="1022" width="11.5185185185185" style="1" customWidth="1"/>
     <col min="1023" max="1024" width="9.13888888888889" style="1" customWidth="1"/>
     <col min="1025" max="16383" width="9.13888888888889" style="1"/>
@@ -6375,6 +6412,2046 @@
       </c>
       <c r="BD29" s="4">
         <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:56">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30">
+        <v>1000</v>
+      </c>
+      <c r="C30">
+        <v>1000</v>
+      </c>
+      <c r="D30">
+        <v>1000</v>
+      </c>
+      <c r="E30">
+        <v>1000</v>
+      </c>
+      <c r="F30">
+        <v>1000</v>
+      </c>
+      <c r="G30">
+        <v>1000</v>
+      </c>
+      <c r="H30">
+        <v>1000</v>
+      </c>
+      <c r="I30">
+        <v>1000</v>
+      </c>
+      <c r="J30">
+        <v>1000</v>
+      </c>
+      <c r="K30">
+        <v>1000</v>
+      </c>
+      <c r="L30">
+        <v>1000</v>
+      </c>
+      <c r="M30">
+        <v>1000</v>
+      </c>
+      <c r="N30">
+        <v>1000</v>
+      </c>
+      <c r="O30">
+        <v>1000</v>
+      </c>
+      <c r="P30">
+        <v>1000</v>
+      </c>
+      <c r="Q30">
+        <v>1000</v>
+      </c>
+      <c r="R30">
+        <v>1000</v>
+      </c>
+      <c r="S30">
+        <v>1000</v>
+      </c>
+      <c r="T30">
+        <v>1000</v>
+      </c>
+      <c r="U30">
+        <v>1000</v>
+      </c>
+      <c r="V30">
+        <v>1000</v>
+      </c>
+      <c r="W30">
+        <v>1000</v>
+      </c>
+      <c r="X30">
+        <v>1000</v>
+      </c>
+      <c r="Y30">
+        <v>1000</v>
+      </c>
+      <c r="Z30">
+        <v>1000</v>
+      </c>
+      <c r="AA30">
+        <v>1000</v>
+      </c>
+      <c r="AB30">
+        <v>1000</v>
+      </c>
+      <c r="AC30">
+        <v>1000</v>
+      </c>
+      <c r="AD30">
+        <v>1000</v>
+      </c>
+      <c r="AE30">
+        <v>1000</v>
+      </c>
+      <c r="AF30">
+        <v>1000</v>
+      </c>
+      <c r="AG30">
+        <v>1000</v>
+      </c>
+      <c r="AH30">
+        <v>1000</v>
+      </c>
+      <c r="AI30">
+        <v>1000</v>
+      </c>
+      <c r="AJ30">
+        <v>1000</v>
+      </c>
+      <c r="AK30">
+        <v>1000</v>
+      </c>
+      <c r="AL30">
+        <v>1000</v>
+      </c>
+      <c r="AM30">
+        <v>1000</v>
+      </c>
+      <c r="AN30">
+        <v>1000</v>
+      </c>
+      <c r="AO30">
+        <v>1000</v>
+      </c>
+      <c r="AP30">
+        <v>1000</v>
+      </c>
+      <c r="AQ30">
+        <v>1000</v>
+      </c>
+      <c r="AR30">
+        <v>1000</v>
+      </c>
+      <c r="AS30">
+        <v>1000</v>
+      </c>
+      <c r="AT30">
+        <v>1000</v>
+      </c>
+      <c r="AU30">
+        <v>1000</v>
+      </c>
+      <c r="AV30">
+        <v>1000</v>
+      </c>
+      <c r="AW30">
+        <v>1000</v>
+      </c>
+      <c r="AX30">
+        <v>1000</v>
+      </c>
+      <c r="AY30">
+        <v>1000</v>
+      </c>
+      <c r="AZ30">
+        <v>1000</v>
+      </c>
+      <c r="BA30">
+        <v>1000</v>
+      </c>
+      <c r="BB30">
+        <v>1000</v>
+      </c>
+      <c r="BC30">
+        <v>1000</v>
+      </c>
+      <c r="BD30">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:56">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31">
+        <v>1000</v>
+      </c>
+      <c r="C31">
+        <v>1000</v>
+      </c>
+      <c r="D31">
+        <v>1000</v>
+      </c>
+      <c r="E31">
+        <v>1000</v>
+      </c>
+      <c r="F31">
+        <v>1000</v>
+      </c>
+      <c r="G31">
+        <v>1000</v>
+      </c>
+      <c r="H31">
+        <v>1000</v>
+      </c>
+      <c r="I31">
+        <v>1000</v>
+      </c>
+      <c r="J31">
+        <v>1000</v>
+      </c>
+      <c r="K31">
+        <v>1000</v>
+      </c>
+      <c r="L31">
+        <v>1000</v>
+      </c>
+      <c r="M31">
+        <v>1000</v>
+      </c>
+      <c r="N31">
+        <v>1000</v>
+      </c>
+      <c r="O31">
+        <v>1000</v>
+      </c>
+      <c r="P31">
+        <v>1000</v>
+      </c>
+      <c r="Q31">
+        <v>1000</v>
+      </c>
+      <c r="R31">
+        <v>1000</v>
+      </c>
+      <c r="S31">
+        <v>1000</v>
+      </c>
+      <c r="T31">
+        <v>1000</v>
+      </c>
+      <c r="U31">
+        <v>1000</v>
+      </c>
+      <c r="V31">
+        <v>1000</v>
+      </c>
+      <c r="W31">
+        <v>1000</v>
+      </c>
+      <c r="X31">
+        <v>1000</v>
+      </c>
+      <c r="Y31">
+        <v>1000</v>
+      </c>
+      <c r="Z31">
+        <v>1000</v>
+      </c>
+      <c r="AA31">
+        <v>1000</v>
+      </c>
+      <c r="AB31">
+        <v>1000</v>
+      </c>
+      <c r="AC31">
+        <v>1000</v>
+      </c>
+      <c r="AD31">
+        <v>1000</v>
+      </c>
+      <c r="AE31">
+        <v>1000</v>
+      </c>
+      <c r="AF31">
+        <v>1000</v>
+      </c>
+      <c r="AG31">
+        <v>1000</v>
+      </c>
+      <c r="AH31">
+        <v>1000</v>
+      </c>
+      <c r="AI31">
+        <v>1000</v>
+      </c>
+      <c r="AJ31">
+        <v>1000</v>
+      </c>
+      <c r="AK31">
+        <v>1000</v>
+      </c>
+      <c r="AL31">
+        <v>1000</v>
+      </c>
+      <c r="AM31">
+        <v>1000</v>
+      </c>
+      <c r="AN31">
+        <v>1000</v>
+      </c>
+      <c r="AO31">
+        <v>1000</v>
+      </c>
+      <c r="AP31">
+        <v>1000</v>
+      </c>
+      <c r="AQ31">
+        <v>1000</v>
+      </c>
+      <c r="AR31">
+        <v>1000</v>
+      </c>
+      <c r="AS31">
+        <v>1000</v>
+      </c>
+      <c r="AT31">
+        <v>1000</v>
+      </c>
+      <c r="AU31">
+        <v>1000</v>
+      </c>
+      <c r="AV31">
+        <v>1000</v>
+      </c>
+      <c r="AW31">
+        <v>1000</v>
+      </c>
+      <c r="AX31">
+        <v>1000</v>
+      </c>
+      <c r="AY31">
+        <v>1000</v>
+      </c>
+      <c r="AZ31">
+        <v>1000</v>
+      </c>
+      <c r="BA31">
+        <v>1000</v>
+      </c>
+      <c r="BB31">
+        <v>1000</v>
+      </c>
+      <c r="BC31">
+        <v>1000</v>
+      </c>
+      <c r="BD31">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:56">
+      <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32">
+        <v>1000</v>
+      </c>
+      <c r="C32">
+        <v>1000</v>
+      </c>
+      <c r="D32">
+        <v>1000</v>
+      </c>
+      <c r="E32">
+        <v>1000</v>
+      </c>
+      <c r="F32">
+        <v>1000</v>
+      </c>
+      <c r="G32">
+        <v>1000</v>
+      </c>
+      <c r="H32">
+        <v>1000</v>
+      </c>
+      <c r="I32">
+        <v>1000</v>
+      </c>
+      <c r="J32">
+        <v>1000</v>
+      </c>
+      <c r="K32">
+        <v>1000</v>
+      </c>
+      <c r="L32">
+        <v>1000</v>
+      </c>
+      <c r="M32">
+        <v>1000</v>
+      </c>
+      <c r="N32">
+        <v>1000</v>
+      </c>
+      <c r="O32">
+        <v>1000</v>
+      </c>
+      <c r="P32">
+        <v>1000</v>
+      </c>
+      <c r="Q32">
+        <v>1000</v>
+      </c>
+      <c r="R32">
+        <v>1000</v>
+      </c>
+      <c r="S32">
+        <v>1000</v>
+      </c>
+      <c r="T32">
+        <v>1000</v>
+      </c>
+      <c r="U32">
+        <v>1000</v>
+      </c>
+      <c r="V32">
+        <v>1000</v>
+      </c>
+      <c r="W32">
+        <v>1000</v>
+      </c>
+      <c r="X32">
+        <v>1000</v>
+      </c>
+      <c r="Y32">
+        <v>1000</v>
+      </c>
+      <c r="Z32">
+        <v>1000</v>
+      </c>
+      <c r="AA32">
+        <v>1000</v>
+      </c>
+      <c r="AB32">
+        <v>1000</v>
+      </c>
+      <c r="AC32">
+        <v>1000</v>
+      </c>
+      <c r="AD32">
+        <v>1000</v>
+      </c>
+      <c r="AE32">
+        <v>1000</v>
+      </c>
+      <c r="AF32">
+        <v>1000</v>
+      </c>
+      <c r="AG32">
+        <v>1000</v>
+      </c>
+      <c r="AH32">
+        <v>1000</v>
+      </c>
+      <c r="AI32">
+        <v>1000</v>
+      </c>
+      <c r="AJ32">
+        <v>1000</v>
+      </c>
+      <c r="AK32">
+        <v>1000</v>
+      </c>
+      <c r="AL32">
+        <v>1000</v>
+      </c>
+      <c r="AM32">
+        <v>1000</v>
+      </c>
+      <c r="AN32">
+        <v>1000</v>
+      </c>
+      <c r="AO32">
+        <v>1000</v>
+      </c>
+      <c r="AP32">
+        <v>1000</v>
+      </c>
+      <c r="AQ32">
+        <v>1000</v>
+      </c>
+      <c r="AR32">
+        <v>1000</v>
+      </c>
+      <c r="AS32">
+        <v>1000</v>
+      </c>
+      <c r="AT32">
+        <v>1000</v>
+      </c>
+      <c r="AU32">
+        <v>1000</v>
+      </c>
+      <c r="AV32">
+        <v>1000</v>
+      </c>
+      <c r="AW32">
+        <v>1000</v>
+      </c>
+      <c r="AX32">
+        <v>1000</v>
+      </c>
+      <c r="AY32">
+        <v>1000</v>
+      </c>
+      <c r="AZ32">
+        <v>1000</v>
+      </c>
+      <c r="BA32">
+        <v>1000</v>
+      </c>
+      <c r="BB32">
+        <v>1000</v>
+      </c>
+      <c r="BC32">
+        <v>1000</v>
+      </c>
+      <c r="BD32">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:56">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33">
+        <v>1000</v>
+      </c>
+      <c r="C33">
+        <v>1000</v>
+      </c>
+      <c r="D33">
+        <v>1000</v>
+      </c>
+      <c r="E33">
+        <v>1000</v>
+      </c>
+      <c r="F33">
+        <v>1000</v>
+      </c>
+      <c r="G33">
+        <v>1000</v>
+      </c>
+      <c r="H33">
+        <v>1000</v>
+      </c>
+      <c r="I33">
+        <v>1000</v>
+      </c>
+      <c r="J33">
+        <v>1000</v>
+      </c>
+      <c r="K33">
+        <v>1000</v>
+      </c>
+      <c r="L33">
+        <v>1000</v>
+      </c>
+      <c r="M33">
+        <v>1000</v>
+      </c>
+      <c r="N33">
+        <v>1000</v>
+      </c>
+      <c r="O33">
+        <v>1000</v>
+      </c>
+      <c r="P33">
+        <v>1000</v>
+      </c>
+      <c r="Q33">
+        <v>1000</v>
+      </c>
+      <c r="R33">
+        <v>1000</v>
+      </c>
+      <c r="S33">
+        <v>1000</v>
+      </c>
+      <c r="T33">
+        <v>1000</v>
+      </c>
+      <c r="U33">
+        <v>1000</v>
+      </c>
+      <c r="V33">
+        <v>1000</v>
+      </c>
+      <c r="W33">
+        <v>1000</v>
+      </c>
+      <c r="X33">
+        <v>1000</v>
+      </c>
+      <c r="Y33">
+        <v>1000</v>
+      </c>
+      <c r="Z33">
+        <v>1000</v>
+      </c>
+      <c r="AA33">
+        <v>1000</v>
+      </c>
+      <c r="AB33">
+        <v>1000</v>
+      </c>
+      <c r="AC33">
+        <v>1000</v>
+      </c>
+      <c r="AD33">
+        <v>1000</v>
+      </c>
+      <c r="AE33">
+        <v>1000</v>
+      </c>
+      <c r="AF33">
+        <v>1000</v>
+      </c>
+      <c r="AG33">
+        <v>1000</v>
+      </c>
+      <c r="AH33">
+        <v>1000</v>
+      </c>
+      <c r="AI33">
+        <v>1000</v>
+      </c>
+      <c r="AJ33">
+        <v>1000</v>
+      </c>
+      <c r="AK33">
+        <v>1000</v>
+      </c>
+      <c r="AL33">
+        <v>1000</v>
+      </c>
+      <c r="AM33">
+        <v>1000</v>
+      </c>
+      <c r="AN33">
+        <v>1000</v>
+      </c>
+      <c r="AO33">
+        <v>1000</v>
+      </c>
+      <c r="AP33">
+        <v>1000</v>
+      </c>
+      <c r="AQ33">
+        <v>1000</v>
+      </c>
+      <c r="AR33">
+        <v>1000</v>
+      </c>
+      <c r="AS33">
+        <v>1000</v>
+      </c>
+      <c r="AT33">
+        <v>1000</v>
+      </c>
+      <c r="AU33">
+        <v>1000</v>
+      </c>
+      <c r="AV33">
+        <v>1000</v>
+      </c>
+      <c r="AW33">
+        <v>1000</v>
+      </c>
+      <c r="AX33">
+        <v>1000</v>
+      </c>
+      <c r="AY33">
+        <v>1000</v>
+      </c>
+      <c r="AZ33">
+        <v>1000</v>
+      </c>
+      <c r="BA33">
+        <v>1000</v>
+      </c>
+      <c r="BB33">
+        <v>1000</v>
+      </c>
+      <c r="BC33">
+        <v>1000</v>
+      </c>
+      <c r="BD33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:56">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34">
+        <v>1000</v>
+      </c>
+      <c r="C34">
+        <v>1000</v>
+      </c>
+      <c r="D34">
+        <v>1000</v>
+      </c>
+      <c r="E34">
+        <v>1000</v>
+      </c>
+      <c r="F34">
+        <v>1000</v>
+      </c>
+      <c r="G34">
+        <v>1000</v>
+      </c>
+      <c r="H34">
+        <v>1000</v>
+      </c>
+      <c r="I34">
+        <v>1000</v>
+      </c>
+      <c r="J34">
+        <v>1000</v>
+      </c>
+      <c r="K34">
+        <v>1000</v>
+      </c>
+      <c r="L34">
+        <v>1000</v>
+      </c>
+      <c r="M34">
+        <v>1000</v>
+      </c>
+      <c r="N34">
+        <v>1000</v>
+      </c>
+      <c r="O34">
+        <v>1000</v>
+      </c>
+      <c r="P34">
+        <v>1000</v>
+      </c>
+      <c r="Q34">
+        <v>1000</v>
+      </c>
+      <c r="R34">
+        <v>1000</v>
+      </c>
+      <c r="S34">
+        <v>1000</v>
+      </c>
+      <c r="T34">
+        <v>1000</v>
+      </c>
+      <c r="U34">
+        <v>1000</v>
+      </c>
+      <c r="V34">
+        <v>1000</v>
+      </c>
+      <c r="W34">
+        <v>1000</v>
+      </c>
+      <c r="X34">
+        <v>1000</v>
+      </c>
+      <c r="Y34">
+        <v>1000</v>
+      </c>
+      <c r="Z34">
+        <v>1000</v>
+      </c>
+      <c r="AA34">
+        <v>1000</v>
+      </c>
+      <c r="AB34">
+        <v>1000</v>
+      </c>
+      <c r="AC34">
+        <v>1000</v>
+      </c>
+      <c r="AD34">
+        <v>1000</v>
+      </c>
+      <c r="AE34">
+        <v>1000</v>
+      </c>
+      <c r="AF34">
+        <v>1000</v>
+      </c>
+      <c r="AG34">
+        <v>1000</v>
+      </c>
+      <c r="AH34">
+        <v>1000</v>
+      </c>
+      <c r="AI34">
+        <v>1000</v>
+      </c>
+      <c r="AJ34">
+        <v>1000</v>
+      </c>
+      <c r="AK34">
+        <v>1000</v>
+      </c>
+      <c r="AL34">
+        <v>1000</v>
+      </c>
+      <c r="AM34">
+        <v>1000</v>
+      </c>
+      <c r="AN34">
+        <v>1000</v>
+      </c>
+      <c r="AO34">
+        <v>1000</v>
+      </c>
+      <c r="AP34">
+        <v>1000</v>
+      </c>
+      <c r="AQ34">
+        <v>1000</v>
+      </c>
+      <c r="AR34">
+        <v>1000</v>
+      </c>
+      <c r="AS34">
+        <v>1000</v>
+      </c>
+      <c r="AT34">
+        <v>1000</v>
+      </c>
+      <c r="AU34">
+        <v>1000</v>
+      </c>
+      <c r="AV34">
+        <v>1000</v>
+      </c>
+      <c r="AW34">
+        <v>1000</v>
+      </c>
+      <c r="AX34">
+        <v>1000</v>
+      </c>
+      <c r="AY34">
+        <v>1000</v>
+      </c>
+      <c r="AZ34">
+        <v>1000</v>
+      </c>
+      <c r="BA34">
+        <v>1000</v>
+      </c>
+      <c r="BB34">
+        <v>1000</v>
+      </c>
+      <c r="BC34">
+        <v>1000</v>
+      </c>
+      <c r="BD34">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:56">
+      <c r="A35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35">
+        <v>1000</v>
+      </c>
+      <c r="C35">
+        <v>1000</v>
+      </c>
+      <c r="D35">
+        <v>1000</v>
+      </c>
+      <c r="E35">
+        <v>1000</v>
+      </c>
+      <c r="F35">
+        <v>1000</v>
+      </c>
+      <c r="G35">
+        <v>1000</v>
+      </c>
+      <c r="H35">
+        <v>1000</v>
+      </c>
+      <c r="I35">
+        <v>1000</v>
+      </c>
+      <c r="J35">
+        <v>1000</v>
+      </c>
+      <c r="K35">
+        <v>1000</v>
+      </c>
+      <c r="L35">
+        <v>1000</v>
+      </c>
+      <c r="M35">
+        <v>1000</v>
+      </c>
+      <c r="N35">
+        <v>1000</v>
+      </c>
+      <c r="O35">
+        <v>1000</v>
+      </c>
+      <c r="P35">
+        <v>1000</v>
+      </c>
+      <c r="Q35">
+        <v>1000</v>
+      </c>
+      <c r="R35">
+        <v>1000</v>
+      </c>
+      <c r="S35">
+        <v>1000</v>
+      </c>
+      <c r="T35">
+        <v>1000</v>
+      </c>
+      <c r="U35">
+        <v>1000</v>
+      </c>
+      <c r="V35">
+        <v>1000</v>
+      </c>
+      <c r="W35">
+        <v>1000</v>
+      </c>
+      <c r="X35">
+        <v>1000</v>
+      </c>
+      <c r="Y35">
+        <v>1000</v>
+      </c>
+      <c r="Z35">
+        <v>1000</v>
+      </c>
+      <c r="AA35">
+        <v>1000</v>
+      </c>
+      <c r="AB35">
+        <v>1000</v>
+      </c>
+      <c r="AC35">
+        <v>1000</v>
+      </c>
+      <c r="AD35">
+        <v>1000</v>
+      </c>
+      <c r="AE35">
+        <v>1000</v>
+      </c>
+      <c r="AF35">
+        <v>1000</v>
+      </c>
+      <c r="AG35">
+        <v>1000</v>
+      </c>
+      <c r="AH35">
+        <v>1000</v>
+      </c>
+      <c r="AI35">
+        <v>1000</v>
+      </c>
+      <c r="AJ35">
+        <v>1000</v>
+      </c>
+      <c r="AK35">
+        <v>1000</v>
+      </c>
+      <c r="AL35">
+        <v>1000</v>
+      </c>
+      <c r="AM35">
+        <v>1000</v>
+      </c>
+      <c r="AN35">
+        <v>1000</v>
+      </c>
+      <c r="AO35">
+        <v>1000</v>
+      </c>
+      <c r="AP35">
+        <v>1000</v>
+      </c>
+      <c r="AQ35">
+        <v>1000</v>
+      </c>
+      <c r="AR35">
+        <v>1000</v>
+      </c>
+      <c r="AS35">
+        <v>1000</v>
+      </c>
+      <c r="AT35">
+        <v>1000</v>
+      </c>
+      <c r="AU35">
+        <v>1000</v>
+      </c>
+      <c r="AV35">
+        <v>1000</v>
+      </c>
+      <c r="AW35">
+        <v>1000</v>
+      </c>
+      <c r="AX35">
+        <v>1000</v>
+      </c>
+      <c r="AY35">
+        <v>1000</v>
+      </c>
+      <c r="AZ35">
+        <v>1000</v>
+      </c>
+      <c r="BA35">
+        <v>1000</v>
+      </c>
+      <c r="BB35">
+        <v>1000</v>
+      </c>
+      <c r="BC35">
+        <v>1000</v>
+      </c>
+      <c r="BD35">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:56">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36">
+        <v>1000</v>
+      </c>
+      <c r="C36">
+        <v>1000</v>
+      </c>
+      <c r="D36">
+        <v>1000</v>
+      </c>
+      <c r="E36">
+        <v>1000</v>
+      </c>
+      <c r="F36">
+        <v>1000</v>
+      </c>
+      <c r="G36">
+        <v>1000</v>
+      </c>
+      <c r="H36">
+        <v>1000</v>
+      </c>
+      <c r="I36">
+        <v>1000</v>
+      </c>
+      <c r="J36">
+        <v>1000</v>
+      </c>
+      <c r="K36">
+        <v>1000</v>
+      </c>
+      <c r="L36">
+        <v>1000</v>
+      </c>
+      <c r="M36">
+        <v>1000</v>
+      </c>
+      <c r="N36">
+        <v>1000</v>
+      </c>
+      <c r="O36">
+        <v>1000</v>
+      </c>
+      <c r="P36">
+        <v>1000</v>
+      </c>
+      <c r="Q36">
+        <v>1000</v>
+      </c>
+      <c r="R36">
+        <v>1000</v>
+      </c>
+      <c r="S36">
+        <v>1000</v>
+      </c>
+      <c r="T36">
+        <v>1000</v>
+      </c>
+      <c r="U36">
+        <v>1000</v>
+      </c>
+      <c r="V36">
+        <v>1000</v>
+      </c>
+      <c r="W36">
+        <v>1000</v>
+      </c>
+      <c r="X36">
+        <v>1000</v>
+      </c>
+      <c r="Y36">
+        <v>1000</v>
+      </c>
+      <c r="Z36">
+        <v>1000</v>
+      </c>
+      <c r="AA36">
+        <v>1000</v>
+      </c>
+      <c r="AB36">
+        <v>1000</v>
+      </c>
+      <c r="AC36">
+        <v>1000</v>
+      </c>
+      <c r="AD36">
+        <v>1000</v>
+      </c>
+      <c r="AE36">
+        <v>1000</v>
+      </c>
+      <c r="AF36">
+        <v>1000</v>
+      </c>
+      <c r="AG36">
+        <v>1000</v>
+      </c>
+      <c r="AH36">
+        <v>1000</v>
+      </c>
+      <c r="AI36">
+        <v>1000</v>
+      </c>
+      <c r="AJ36">
+        <v>1000</v>
+      </c>
+      <c r="AK36">
+        <v>1000</v>
+      </c>
+      <c r="AL36">
+        <v>1000</v>
+      </c>
+      <c r="AM36">
+        <v>1000</v>
+      </c>
+      <c r="AN36">
+        <v>1000</v>
+      </c>
+      <c r="AO36">
+        <v>1000</v>
+      </c>
+      <c r="AP36">
+        <v>1000</v>
+      </c>
+      <c r="AQ36">
+        <v>1000</v>
+      </c>
+      <c r="AR36">
+        <v>1000</v>
+      </c>
+      <c r="AS36">
+        <v>1000</v>
+      </c>
+      <c r="AT36">
+        <v>1000</v>
+      </c>
+      <c r="AU36">
+        <v>1000</v>
+      </c>
+      <c r="AV36">
+        <v>1000</v>
+      </c>
+      <c r="AW36">
+        <v>1000</v>
+      </c>
+      <c r="AX36">
+        <v>1000</v>
+      </c>
+      <c r="AY36">
+        <v>1000</v>
+      </c>
+      <c r="AZ36">
+        <v>1000</v>
+      </c>
+      <c r="BA36">
+        <v>1000</v>
+      </c>
+      <c r="BB36">
+        <v>1000</v>
+      </c>
+      <c r="BC36">
+        <v>1000</v>
+      </c>
+      <c r="BD36">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:56">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37">
+        <v>1000</v>
+      </c>
+      <c r="C37">
+        <v>1000</v>
+      </c>
+      <c r="D37">
+        <v>1000</v>
+      </c>
+      <c r="E37">
+        <v>1000</v>
+      </c>
+      <c r="F37">
+        <v>1000</v>
+      </c>
+      <c r="G37">
+        <v>1000</v>
+      </c>
+      <c r="H37">
+        <v>1000</v>
+      </c>
+      <c r="I37">
+        <v>1000</v>
+      </c>
+      <c r="J37">
+        <v>1000</v>
+      </c>
+      <c r="K37">
+        <v>1000</v>
+      </c>
+      <c r="L37">
+        <v>1000</v>
+      </c>
+      <c r="M37">
+        <v>1000</v>
+      </c>
+      <c r="N37">
+        <v>1000</v>
+      </c>
+      <c r="O37">
+        <v>1000</v>
+      </c>
+      <c r="P37">
+        <v>1000</v>
+      </c>
+      <c r="Q37">
+        <v>1000</v>
+      </c>
+      <c r="R37">
+        <v>1000</v>
+      </c>
+      <c r="S37">
+        <v>1000</v>
+      </c>
+      <c r="T37">
+        <v>1000</v>
+      </c>
+      <c r="U37">
+        <v>1000</v>
+      </c>
+      <c r="V37">
+        <v>1000</v>
+      </c>
+      <c r="W37">
+        <v>1000</v>
+      </c>
+      <c r="X37">
+        <v>1000</v>
+      </c>
+      <c r="Y37">
+        <v>1000</v>
+      </c>
+      <c r="Z37">
+        <v>1000</v>
+      </c>
+      <c r="AA37">
+        <v>1000</v>
+      </c>
+      <c r="AB37">
+        <v>1000</v>
+      </c>
+      <c r="AC37">
+        <v>1000</v>
+      </c>
+      <c r="AD37">
+        <v>1000</v>
+      </c>
+      <c r="AE37">
+        <v>1000</v>
+      </c>
+      <c r="AF37">
+        <v>1000</v>
+      </c>
+      <c r="AG37">
+        <v>1000</v>
+      </c>
+      <c r="AH37">
+        <v>1000</v>
+      </c>
+      <c r="AI37">
+        <v>1000</v>
+      </c>
+      <c r="AJ37">
+        <v>1000</v>
+      </c>
+      <c r="AK37">
+        <v>1000</v>
+      </c>
+      <c r="AL37">
+        <v>1000</v>
+      </c>
+      <c r="AM37">
+        <v>1000</v>
+      </c>
+      <c r="AN37">
+        <v>1000</v>
+      </c>
+      <c r="AO37">
+        <v>1000</v>
+      </c>
+      <c r="AP37">
+        <v>1000</v>
+      </c>
+      <c r="AQ37">
+        <v>1000</v>
+      </c>
+      <c r="AR37">
+        <v>1000</v>
+      </c>
+      <c r="AS37">
+        <v>1000</v>
+      </c>
+      <c r="AT37">
+        <v>1000</v>
+      </c>
+      <c r="AU37">
+        <v>1000</v>
+      </c>
+      <c r="AV37">
+        <v>1000</v>
+      </c>
+      <c r="AW37">
+        <v>1000</v>
+      </c>
+      <c r="AX37">
+        <v>1000</v>
+      </c>
+      <c r="AY37">
+        <v>1000</v>
+      </c>
+      <c r="AZ37">
+        <v>1000</v>
+      </c>
+      <c r="BA37">
+        <v>1000</v>
+      </c>
+      <c r="BB37">
+        <v>1000</v>
+      </c>
+      <c r="BC37">
+        <v>1000</v>
+      </c>
+      <c r="BD37">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:56">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38">
+        <v>1000</v>
+      </c>
+      <c r="C38">
+        <v>1000</v>
+      </c>
+      <c r="D38">
+        <v>1000</v>
+      </c>
+      <c r="E38">
+        <v>1000</v>
+      </c>
+      <c r="F38">
+        <v>1000</v>
+      </c>
+      <c r="G38">
+        <v>1000</v>
+      </c>
+      <c r="H38">
+        <v>1000</v>
+      </c>
+      <c r="I38">
+        <v>1000</v>
+      </c>
+      <c r="J38">
+        <v>1000</v>
+      </c>
+      <c r="K38">
+        <v>1000</v>
+      </c>
+      <c r="L38">
+        <v>1000</v>
+      </c>
+      <c r="M38">
+        <v>1000</v>
+      </c>
+      <c r="N38">
+        <v>1000</v>
+      </c>
+      <c r="O38">
+        <v>1000</v>
+      </c>
+      <c r="P38">
+        <v>1000</v>
+      </c>
+      <c r="Q38">
+        <v>1000</v>
+      </c>
+      <c r="R38">
+        <v>1000</v>
+      </c>
+      <c r="S38">
+        <v>1000</v>
+      </c>
+      <c r="T38">
+        <v>1000</v>
+      </c>
+      <c r="U38">
+        <v>1000</v>
+      </c>
+      <c r="V38">
+        <v>1000</v>
+      </c>
+      <c r="W38">
+        <v>1000</v>
+      </c>
+      <c r="X38">
+        <v>1000</v>
+      </c>
+      <c r="Y38">
+        <v>1000</v>
+      </c>
+      <c r="Z38">
+        <v>1000</v>
+      </c>
+      <c r="AA38">
+        <v>1000</v>
+      </c>
+      <c r="AB38">
+        <v>1000</v>
+      </c>
+      <c r="AC38">
+        <v>1000</v>
+      </c>
+      <c r="AD38">
+        <v>1000</v>
+      </c>
+      <c r="AE38">
+        <v>1000</v>
+      </c>
+      <c r="AF38">
+        <v>1000</v>
+      </c>
+      <c r="AG38">
+        <v>1000</v>
+      </c>
+      <c r="AH38">
+        <v>1000</v>
+      </c>
+      <c r="AI38">
+        <v>1000</v>
+      </c>
+      <c r="AJ38">
+        <v>1000</v>
+      </c>
+      <c r="AK38">
+        <v>1000</v>
+      </c>
+      <c r="AL38">
+        <v>1000</v>
+      </c>
+      <c r="AM38">
+        <v>1000</v>
+      </c>
+      <c r="AN38">
+        <v>1000</v>
+      </c>
+      <c r="AO38">
+        <v>1000</v>
+      </c>
+      <c r="AP38">
+        <v>1000</v>
+      </c>
+      <c r="AQ38">
+        <v>1000</v>
+      </c>
+      <c r="AR38">
+        <v>1000</v>
+      </c>
+      <c r="AS38">
+        <v>1000</v>
+      </c>
+      <c r="AT38">
+        <v>1000</v>
+      </c>
+      <c r="AU38">
+        <v>1000</v>
+      </c>
+      <c r="AV38">
+        <v>1000</v>
+      </c>
+      <c r="AW38">
+        <v>1000</v>
+      </c>
+      <c r="AX38">
+        <v>1000</v>
+      </c>
+      <c r="AY38">
+        <v>1000</v>
+      </c>
+      <c r="AZ38">
+        <v>1000</v>
+      </c>
+      <c r="BA38">
+        <v>1000</v>
+      </c>
+      <c r="BB38">
+        <v>1000</v>
+      </c>
+      <c r="BC38">
+        <v>1000</v>
+      </c>
+      <c r="BD38">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:56">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39">
+        <v>1000</v>
+      </c>
+      <c r="C39">
+        <v>1000</v>
+      </c>
+      <c r="D39">
+        <v>1000</v>
+      </c>
+      <c r="E39">
+        <v>1000</v>
+      </c>
+      <c r="F39">
+        <v>1000</v>
+      </c>
+      <c r="G39">
+        <v>1000</v>
+      </c>
+      <c r="H39">
+        <v>1000</v>
+      </c>
+      <c r="I39">
+        <v>1000</v>
+      </c>
+      <c r="J39">
+        <v>1000</v>
+      </c>
+      <c r="K39">
+        <v>1000</v>
+      </c>
+      <c r="L39">
+        <v>1000</v>
+      </c>
+      <c r="M39">
+        <v>1000</v>
+      </c>
+      <c r="N39">
+        <v>1000</v>
+      </c>
+      <c r="O39">
+        <v>1000</v>
+      </c>
+      <c r="P39">
+        <v>1000</v>
+      </c>
+      <c r="Q39">
+        <v>1000</v>
+      </c>
+      <c r="R39">
+        <v>1000</v>
+      </c>
+      <c r="S39">
+        <v>1000</v>
+      </c>
+      <c r="T39">
+        <v>1000</v>
+      </c>
+      <c r="U39">
+        <v>1000</v>
+      </c>
+      <c r="V39">
+        <v>1000</v>
+      </c>
+      <c r="W39">
+        <v>1000</v>
+      </c>
+      <c r="X39">
+        <v>1000</v>
+      </c>
+      <c r="Y39">
+        <v>1000</v>
+      </c>
+      <c r="Z39">
+        <v>1000</v>
+      </c>
+      <c r="AA39">
+        <v>1000</v>
+      </c>
+      <c r="AB39">
+        <v>1000</v>
+      </c>
+      <c r="AC39">
+        <v>1000</v>
+      </c>
+      <c r="AD39">
+        <v>1000</v>
+      </c>
+      <c r="AE39">
+        <v>1000</v>
+      </c>
+      <c r="AF39">
+        <v>1000</v>
+      </c>
+      <c r="AG39">
+        <v>1000</v>
+      </c>
+      <c r="AH39">
+        <v>1000</v>
+      </c>
+      <c r="AI39">
+        <v>1000</v>
+      </c>
+      <c r="AJ39">
+        <v>1000</v>
+      </c>
+      <c r="AK39">
+        <v>1000</v>
+      </c>
+      <c r="AL39">
+        <v>1000</v>
+      </c>
+      <c r="AM39">
+        <v>1000</v>
+      </c>
+      <c r="AN39">
+        <v>1000</v>
+      </c>
+      <c r="AO39">
+        <v>1000</v>
+      </c>
+      <c r="AP39">
+        <v>1000</v>
+      </c>
+      <c r="AQ39">
+        <v>1000</v>
+      </c>
+      <c r="AR39">
+        <v>1000</v>
+      </c>
+      <c r="AS39">
+        <v>1000</v>
+      </c>
+      <c r="AT39">
+        <v>1000</v>
+      </c>
+      <c r="AU39">
+        <v>1000</v>
+      </c>
+      <c r="AV39">
+        <v>1000</v>
+      </c>
+      <c r="AW39">
+        <v>1000</v>
+      </c>
+      <c r="AX39">
+        <v>1000</v>
+      </c>
+      <c r="AY39">
+        <v>1000</v>
+      </c>
+      <c r="AZ39">
+        <v>1000</v>
+      </c>
+      <c r="BA39">
+        <v>1000</v>
+      </c>
+      <c r="BB39">
+        <v>1000</v>
+      </c>
+      <c r="BC39">
+        <v>1000</v>
+      </c>
+      <c r="BD39">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:56">
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40">
+        <v>1000</v>
+      </c>
+      <c r="C40">
+        <v>1000</v>
+      </c>
+      <c r="D40">
+        <v>1000</v>
+      </c>
+      <c r="E40">
+        <v>1000</v>
+      </c>
+      <c r="F40">
+        <v>1000</v>
+      </c>
+      <c r="G40">
+        <v>1000</v>
+      </c>
+      <c r="H40">
+        <v>1000</v>
+      </c>
+      <c r="I40">
+        <v>1000</v>
+      </c>
+      <c r="J40">
+        <v>1000</v>
+      </c>
+      <c r="K40">
+        <v>1000</v>
+      </c>
+      <c r="L40">
+        <v>1000</v>
+      </c>
+      <c r="M40">
+        <v>1000</v>
+      </c>
+      <c r="N40">
+        <v>1000</v>
+      </c>
+      <c r="O40">
+        <v>1000</v>
+      </c>
+      <c r="P40">
+        <v>1000</v>
+      </c>
+      <c r="Q40">
+        <v>1000</v>
+      </c>
+      <c r="R40">
+        <v>1000</v>
+      </c>
+      <c r="S40">
+        <v>1000</v>
+      </c>
+      <c r="T40">
+        <v>1000</v>
+      </c>
+      <c r="U40">
+        <v>1000</v>
+      </c>
+      <c r="V40">
+        <v>1000</v>
+      </c>
+      <c r="W40">
+        <v>1000</v>
+      </c>
+      <c r="X40">
+        <v>1000</v>
+      </c>
+      <c r="Y40">
+        <v>1000</v>
+      </c>
+      <c r="Z40">
+        <v>1000</v>
+      </c>
+      <c r="AA40">
+        <v>1000</v>
+      </c>
+      <c r="AB40">
+        <v>1000</v>
+      </c>
+      <c r="AC40">
+        <v>1000</v>
+      </c>
+      <c r="AD40">
+        <v>1000</v>
+      </c>
+      <c r="AE40">
+        <v>1000</v>
+      </c>
+      <c r="AF40">
+        <v>1000</v>
+      </c>
+      <c r="AG40">
+        <v>1000</v>
+      </c>
+      <c r="AH40">
+        <v>1000</v>
+      </c>
+      <c r="AI40">
+        <v>1000</v>
+      </c>
+      <c r="AJ40">
+        <v>1000</v>
+      </c>
+      <c r="AK40">
+        <v>1000</v>
+      </c>
+      <c r="AL40">
+        <v>1000</v>
+      </c>
+      <c r="AM40">
+        <v>1000</v>
+      </c>
+      <c r="AN40">
+        <v>1000</v>
+      </c>
+      <c r="AO40">
+        <v>1000</v>
+      </c>
+      <c r="AP40">
+        <v>1000</v>
+      </c>
+      <c r="AQ40">
+        <v>1000</v>
+      </c>
+      <c r="AR40">
+        <v>1000</v>
+      </c>
+      <c r="AS40">
+        <v>1000</v>
+      </c>
+      <c r="AT40">
+        <v>1000</v>
+      </c>
+      <c r="AU40">
+        <v>1000</v>
+      </c>
+      <c r="AV40">
+        <v>1000</v>
+      </c>
+      <c r="AW40">
+        <v>1000</v>
+      </c>
+      <c r="AX40">
+        <v>1000</v>
+      </c>
+      <c r="AY40">
+        <v>1000</v>
+      </c>
+      <c r="AZ40">
+        <v>1000</v>
+      </c>
+      <c r="BA40">
+        <v>1000</v>
+      </c>
+      <c r="BB40">
+        <v>1000</v>
+      </c>
+      <c r="BC40">
+        <v>1000</v>
+      </c>
+      <c r="BD40">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:56">
+      <c r="A41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41">
+        <v>1000</v>
+      </c>
+      <c r="C41">
+        <v>1000</v>
+      </c>
+      <c r="D41">
+        <v>1000</v>
+      </c>
+      <c r="E41">
+        <v>1000</v>
+      </c>
+      <c r="F41">
+        <v>1000</v>
+      </c>
+      <c r="G41">
+        <v>1000</v>
+      </c>
+      <c r="H41">
+        <v>1000</v>
+      </c>
+      <c r="I41">
+        <v>1000</v>
+      </c>
+      <c r="J41">
+        <v>1000</v>
+      </c>
+      <c r="K41">
+        <v>1000</v>
+      </c>
+      <c r="L41">
+        <v>1000</v>
+      </c>
+      <c r="M41">
+        <v>1000</v>
+      </c>
+      <c r="N41">
+        <v>1000</v>
+      </c>
+      <c r="O41">
+        <v>1000</v>
+      </c>
+      <c r="P41">
+        <v>1000</v>
+      </c>
+      <c r="Q41">
+        <v>1000</v>
+      </c>
+      <c r="R41">
+        <v>1000</v>
+      </c>
+      <c r="S41">
+        <v>1000</v>
+      </c>
+      <c r="T41">
+        <v>1000</v>
+      </c>
+      <c r="U41">
+        <v>1000</v>
+      </c>
+      <c r="V41">
+        <v>1000</v>
+      </c>
+      <c r="W41">
+        <v>1000</v>
+      </c>
+      <c r="X41">
+        <v>1000</v>
+      </c>
+      <c r="Y41">
+        <v>1000</v>
+      </c>
+      <c r="Z41">
+        <v>1000</v>
+      </c>
+      <c r="AA41">
+        <v>1000</v>
+      </c>
+      <c r="AB41">
+        <v>1000</v>
+      </c>
+      <c r="AC41">
+        <v>1000</v>
+      </c>
+      <c r="AD41">
+        <v>1000</v>
+      </c>
+      <c r="AE41">
+        <v>1000</v>
+      </c>
+      <c r="AF41">
+        <v>1000</v>
+      </c>
+      <c r="AG41">
+        <v>1000</v>
+      </c>
+      <c r="AH41">
+        <v>1000</v>
+      </c>
+      <c r="AI41">
+        <v>1000</v>
+      </c>
+      <c r="AJ41">
+        <v>1000</v>
+      </c>
+      <c r="AK41">
+        <v>1000</v>
+      </c>
+      <c r="AL41">
+        <v>1000</v>
+      </c>
+      <c r="AM41">
+        <v>1000</v>
+      </c>
+      <c r="AN41">
+        <v>1000</v>
+      </c>
+      <c r="AO41">
+        <v>1000</v>
+      </c>
+      <c r="AP41">
+        <v>1000</v>
+      </c>
+      <c r="AQ41">
+        <v>1000</v>
+      </c>
+      <c r="AR41">
+        <v>1000</v>
+      </c>
+      <c r="AS41">
+        <v>1000</v>
+      </c>
+      <c r="AT41">
+        <v>1000</v>
+      </c>
+      <c r="AU41">
+        <v>1000</v>
+      </c>
+      <c r="AV41">
+        <v>1000</v>
+      </c>
+      <c r="AW41">
+        <v>1000</v>
+      </c>
+      <c r="AX41">
+        <v>1000</v>
+      </c>
+      <c r="AY41">
+        <v>1000</v>
+      </c>
+      <c r="AZ41">
+        <v>1000</v>
+      </c>
+      <c r="BA41">
+        <v>1000</v>
+      </c>
+      <c r="BB41">
+        <v>1000</v>
+      </c>
+      <c r="BC41">
+        <v>1000</v>
+      </c>
+      <c r="BD41">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -6404,18 +8481,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" ht="12.6" spans="1:2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -6423,7 +8500,7 @@
     </row>
     <row r="3" ht="12.6" spans="1:2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -6431,7 +8508,7 @@
     </row>
     <row r="4" ht="12.6" spans="1:2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -6439,7 +8516,7 @@
     </row>
     <row r="5" ht="12.6" spans="1:2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -6447,7 +8524,7 @@
     </row>
     <row r="6" ht="12.6" spans="1:2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -6455,7 +8532,7 @@
     </row>
     <row r="7" ht="12.6" spans="1:2">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -6463,7 +8540,7 @@
     </row>
     <row r="8" ht="12.6" spans="1:2">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -6471,18 +8548,18 @@
     </row>
     <row r="9" ht="12.6" spans="1:3">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" ht="12.6" spans="1:2">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -6490,7 +8567,7 @@
     </row>
     <row r="11" ht="12.6" spans="1:2">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -6498,7 +8575,7 @@
     </row>
     <row r="12" ht="12.6" spans="1:2">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -6506,7 +8583,7 @@
     </row>
     <row r="13" ht="12.6" spans="1:2">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
@@ -6514,7 +8591,7 @@
     </row>
     <row r="14" ht="12.6" spans="1:2">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -6522,7 +8599,7 @@
     </row>
     <row r="15" ht="12.6" spans="1:2">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -6530,7 +8607,7 @@
     </row>
     <row r="16" ht="12.6" spans="1:2">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -6538,18 +8615,18 @@
     </row>
     <row r="17" ht="12.6" spans="1:3">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" ht="12.6" spans="1:2">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -6557,7 +8634,7 @@
     </row>
     <row r="19" ht="12.6" spans="1:2">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -6565,7 +8642,7 @@
     </row>
     <row r="20" ht="12.6" spans="1:2">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -6573,7 +8650,7 @@
     </row>
     <row r="21" ht="12.6" spans="1:2">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
@@ -6581,7 +8658,7 @@
     </row>
     <row r="22" ht="12.6" spans="1:2">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -6589,7 +8666,7 @@
     </row>
     <row r="23" ht="12.6" spans="1:2">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
@@ -6597,7 +8674,7 @@
     </row>
     <row r="24" ht="12.6" spans="1:2">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
@@ -6605,18 +8682,18 @@
     </row>
     <row r="25" ht="12.6" spans="1:3">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" ht="12.6" spans="1:2">
       <c r="A26" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -6624,7 +8701,7 @@
     </row>
     <row r="27" ht="12.6" spans="1:2">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -6632,7 +8709,7 @@
     </row>
     <row r="28" ht="12.6" spans="1:2">
       <c r="A28" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
@@ -6640,7 +8717,7 @@
     </row>
     <row r="29" ht="12.6" spans="1:2">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
@@ -6648,7 +8725,7 @@
     </row>
     <row r="30" ht="12.6" spans="1:2">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -6656,7 +8733,7 @@
     </row>
     <row r="31" ht="12.6" spans="1:2">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -6664,7 +8741,7 @@
     </row>
     <row r="32" ht="12.6" spans="1:2">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
@@ -6672,18 +8749,18 @@
     </row>
     <row r="33" ht="12.6" spans="1:3">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B33" t="s">
         <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" ht="12.6" spans="1:2">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
@@ -6691,7 +8768,7 @@
     </row>
     <row r="35" ht="12.6" spans="1:2">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
@@ -6699,7 +8776,7 @@
     </row>
     <row r="36" ht="12.6" spans="1:2">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
@@ -6707,7 +8784,7 @@
     </row>
     <row r="37" ht="12.6" spans="1:2">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -6715,7 +8792,7 @@
     </row>
     <row r="38" ht="12.6" spans="1:2">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
@@ -6723,7 +8800,7 @@
     </row>
     <row r="39" ht="12.6" spans="1:2">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
@@ -6731,7 +8808,7 @@
     </row>
     <row r="40" ht="12.6" spans="1:2">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="B40" t="s">
         <v>38</v>
@@ -6739,18 +8816,18 @@
     </row>
     <row r="41" ht="12.6" spans="1:3">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="B41" t="s">
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" ht="12.6" spans="1:2">
       <c r="A42" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="B42" t="s">
         <v>40</v>
@@ -6758,7 +8835,7 @@
     </row>
     <row r="43" ht="12.6" spans="1:2">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B43" t="s">
         <v>41</v>
@@ -6766,7 +8843,7 @@
     </row>
     <row r="44" ht="12.6" spans="1:2">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="B44" t="s">
         <v>42</v>
@@ -6774,7 +8851,7 @@
     </row>
     <row r="45" ht="12.6" spans="1:2">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="B45" t="s">
         <v>43</v>
@@ -6782,7 +8859,7 @@
     </row>
     <row r="46" ht="12.6" spans="1:2">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="B46" t="s">
         <v>44</v>
@@ -6790,7 +8867,7 @@
     </row>
     <row r="47" ht="12.6" spans="1:2">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s">
         <v>45</v>
@@ -6798,7 +8875,7 @@
     </row>
     <row r="48" ht="12.6" spans="1:2">
       <c r="A48" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
@@ -6806,18 +8883,18 @@
     </row>
     <row r="49" ht="12.6" spans="1:3">
       <c r="A49" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="B49" t="s">
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" ht="12.6" spans="1:2">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B50" t="s">
         <v>48</v>
@@ -6825,7 +8902,7 @@
     </row>
     <row r="51" ht="12.6" spans="1:2">
       <c r="A51" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
@@ -6833,7 +8910,7 @@
     </row>
     <row r="52" ht="12.6" spans="1:2">
       <c r="A52" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="B52" t="s">
         <v>50</v>
@@ -6841,7 +8918,7 @@
     </row>
     <row r="53" ht="12.6" spans="1:2">
       <c r="A53" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
         <v>51</v>
@@ -6849,7 +8926,7 @@
     </row>
     <row r="54" ht="12.6" spans="1:2">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
@@ -6857,7 +8934,7 @@
     </row>
     <row r="55" ht="12.6" spans="1:2">
       <c r="A55" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="B55" t="s">
         <v>53</v>
@@ -6865,7 +8942,7 @@
     </row>
     <row r="56" ht="12.6" spans="1:2">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Set all detector biases to zero in warm condition
</commit_message>
<xml_diff>
--- a/data/default_biases_warm.xlsx
+++ b/data/default_biases_warm.xlsx
@@ -1470,8 +1470,8 @@
   <sheetPr/>
   <dimension ref="A1:BD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:BD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -6419,169 +6419,169 @@
         <v>84</v>
       </c>
       <c r="B30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC30">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD30">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:56">
@@ -6589,169 +6589,169 @@
         <v>85</v>
       </c>
       <c r="B31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC31">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD31">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:56">
@@ -6759,169 +6759,169 @@
         <v>86</v>
       </c>
       <c r="B32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC32">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD32">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:56">
@@ -6929,169 +6929,169 @@
         <v>87</v>
       </c>
       <c r="B33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC33">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD33">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:56">
@@ -7099,169 +7099,169 @@
         <v>88</v>
       </c>
       <c r="B34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC34">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD34">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:56">
@@ -7269,169 +7269,169 @@
         <v>89</v>
       </c>
       <c r="B35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC35">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD35">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:56">
@@ -7439,169 +7439,169 @@
         <v>90</v>
       </c>
       <c r="B36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD36">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:56">
@@ -7609,169 +7609,169 @@
         <v>91</v>
       </c>
       <c r="B37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC37">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD37">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:56">
@@ -7779,169 +7779,169 @@
         <v>92</v>
       </c>
       <c r="B38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC38">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD38">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:56">
@@ -7949,169 +7949,169 @@
         <v>93</v>
       </c>
       <c r="B39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC39">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD39">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:56">
@@ -8119,169 +8119,169 @@
         <v>94</v>
       </c>
       <c r="B40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC40">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD40">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:56">
@@ -8289,169 +8289,169 @@
         <v>95</v>
       </c>
       <c r="B41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC41">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD41">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set detector parameters in turnon procedure (#80)
* Set offset and gain for detectors in turnon

* Add detectors hks to bias tables (warm/cryo)

* Set proper detector biases in turnon procedure

* Set all detector biases to zero in warm condition
</commit_message>
<xml_diff>
--- a/data/default_biases_warm.xlsx
+++ b/data/default_biases_warm.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="160">
   <si>
     <t>PAR</t>
   </si>
@@ -273,6 +273,42 @@
   </si>
   <si>
     <t>ID5</t>
+  </si>
+  <si>
+    <t>DET0_BIAS</t>
+  </si>
+  <si>
+    <t>DET1_BIAS</t>
+  </si>
+  <si>
+    <t>DET2_BIAS</t>
+  </si>
+  <si>
+    <t>DET3_BIAS</t>
+  </si>
+  <si>
+    <t>DET0_OFFSET</t>
+  </si>
+  <si>
+    <t>DET1_OFFSET</t>
+  </si>
+  <si>
+    <t>DET2_OFFSET</t>
+  </si>
+  <si>
+    <t>DET3_OFFSET</t>
+  </si>
+  <si>
+    <t>DET0_GAIN</t>
+  </si>
+  <si>
+    <t>DET1_GAIN</t>
+  </si>
+  <si>
+    <t>DET2_GAIN</t>
+  </si>
+  <si>
+    <t>DET3_GAIN</t>
   </si>
   <si>
     <t>Module</t>
@@ -473,9 +509,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -511,9 +547,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -527,8 +562,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -541,19 +577,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -572,10 +608,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -587,21 +624,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -610,16 +632,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -634,22 +655,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -664,13 +700,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,102 +736,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -796,7 +748,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,19 +856,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,7 +868,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,7 +880,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -873,15 +909,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -893,6 +920,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -912,11 +948,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -931,177 +991,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1432,15 +1468,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BD29"/>
+  <dimension ref="A1:BD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AV7" sqref="AV7"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:BD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1021" width="8.5462962962963" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8888888888889" style="1" customWidth="1"/>
+    <col min="2" max="1021" width="8.5462962962963" style="1" customWidth="1"/>
     <col min="1022" max="1022" width="11.5185185185185" style="1" customWidth="1"/>
     <col min="1023" max="1024" width="9.13888888888889" style="1" customWidth="1"/>
     <col min="1025" max="16383" width="9.13888888888889" style="1"/>
@@ -6374,6 +6411,2046 @@
         <v>4114</v>
       </c>
       <c r="BD29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:56">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <v>0</v>
+      </c>
+      <c r="AB30">
+        <v>0</v>
+      </c>
+      <c r="AC30">
+        <v>0</v>
+      </c>
+      <c r="AD30">
+        <v>0</v>
+      </c>
+      <c r="AE30">
+        <v>0</v>
+      </c>
+      <c r="AF30">
+        <v>0</v>
+      </c>
+      <c r="AG30">
+        <v>0</v>
+      </c>
+      <c r="AH30">
+        <v>0</v>
+      </c>
+      <c r="AI30">
+        <v>0</v>
+      </c>
+      <c r="AJ30">
+        <v>0</v>
+      </c>
+      <c r="AK30">
+        <v>0</v>
+      </c>
+      <c r="AL30">
+        <v>0</v>
+      </c>
+      <c r="AM30">
+        <v>0</v>
+      </c>
+      <c r="AN30">
+        <v>0</v>
+      </c>
+      <c r="AO30">
+        <v>0</v>
+      </c>
+      <c r="AP30">
+        <v>0</v>
+      </c>
+      <c r="AQ30">
+        <v>0</v>
+      </c>
+      <c r="AR30">
+        <v>0</v>
+      </c>
+      <c r="AS30">
+        <v>0</v>
+      </c>
+      <c r="AT30">
+        <v>0</v>
+      </c>
+      <c r="AU30">
+        <v>0</v>
+      </c>
+      <c r="AV30">
+        <v>0</v>
+      </c>
+      <c r="AW30">
+        <v>0</v>
+      </c>
+      <c r="AX30">
+        <v>0</v>
+      </c>
+      <c r="AY30">
+        <v>0</v>
+      </c>
+      <c r="AZ30">
+        <v>0</v>
+      </c>
+      <c r="BA30">
+        <v>0</v>
+      </c>
+      <c r="BB30">
+        <v>0</v>
+      </c>
+      <c r="BC30">
+        <v>0</v>
+      </c>
+      <c r="BD30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:56">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>0</v>
+      </c>
+      <c r="AA31">
+        <v>0</v>
+      </c>
+      <c r="AB31">
+        <v>0</v>
+      </c>
+      <c r="AC31">
+        <v>0</v>
+      </c>
+      <c r="AD31">
+        <v>0</v>
+      </c>
+      <c r="AE31">
+        <v>0</v>
+      </c>
+      <c r="AF31">
+        <v>0</v>
+      </c>
+      <c r="AG31">
+        <v>0</v>
+      </c>
+      <c r="AH31">
+        <v>0</v>
+      </c>
+      <c r="AI31">
+        <v>0</v>
+      </c>
+      <c r="AJ31">
+        <v>0</v>
+      </c>
+      <c r="AK31">
+        <v>0</v>
+      </c>
+      <c r="AL31">
+        <v>0</v>
+      </c>
+      <c r="AM31">
+        <v>0</v>
+      </c>
+      <c r="AN31">
+        <v>0</v>
+      </c>
+      <c r="AO31">
+        <v>0</v>
+      </c>
+      <c r="AP31">
+        <v>0</v>
+      </c>
+      <c r="AQ31">
+        <v>0</v>
+      </c>
+      <c r="AR31">
+        <v>0</v>
+      </c>
+      <c r="AS31">
+        <v>0</v>
+      </c>
+      <c r="AT31">
+        <v>0</v>
+      </c>
+      <c r="AU31">
+        <v>0</v>
+      </c>
+      <c r="AV31">
+        <v>0</v>
+      </c>
+      <c r="AW31">
+        <v>0</v>
+      </c>
+      <c r="AX31">
+        <v>0</v>
+      </c>
+      <c r="AY31">
+        <v>0</v>
+      </c>
+      <c r="AZ31">
+        <v>0</v>
+      </c>
+      <c r="BA31">
+        <v>0</v>
+      </c>
+      <c r="BB31">
+        <v>0</v>
+      </c>
+      <c r="BC31">
+        <v>0</v>
+      </c>
+      <c r="BD31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:56">
+      <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <v>0</v>
+      </c>
+      <c r="AC32">
+        <v>0</v>
+      </c>
+      <c r="AD32">
+        <v>0</v>
+      </c>
+      <c r="AE32">
+        <v>0</v>
+      </c>
+      <c r="AF32">
+        <v>0</v>
+      </c>
+      <c r="AG32">
+        <v>0</v>
+      </c>
+      <c r="AH32">
+        <v>0</v>
+      </c>
+      <c r="AI32">
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <v>0</v>
+      </c>
+      <c r="AK32">
+        <v>0</v>
+      </c>
+      <c r="AL32">
+        <v>0</v>
+      </c>
+      <c r="AM32">
+        <v>0</v>
+      </c>
+      <c r="AN32">
+        <v>0</v>
+      </c>
+      <c r="AO32">
+        <v>0</v>
+      </c>
+      <c r="AP32">
+        <v>0</v>
+      </c>
+      <c r="AQ32">
+        <v>0</v>
+      </c>
+      <c r="AR32">
+        <v>0</v>
+      </c>
+      <c r="AS32">
+        <v>0</v>
+      </c>
+      <c r="AT32">
+        <v>0</v>
+      </c>
+      <c r="AU32">
+        <v>0</v>
+      </c>
+      <c r="AV32">
+        <v>0</v>
+      </c>
+      <c r="AW32">
+        <v>0</v>
+      </c>
+      <c r="AX32">
+        <v>0</v>
+      </c>
+      <c r="AY32">
+        <v>0</v>
+      </c>
+      <c r="AZ32">
+        <v>0</v>
+      </c>
+      <c r="BA32">
+        <v>0</v>
+      </c>
+      <c r="BB32">
+        <v>0</v>
+      </c>
+      <c r="BC32">
+        <v>0</v>
+      </c>
+      <c r="BD32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:56">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>0</v>
+      </c>
+      <c r="AB33">
+        <v>0</v>
+      </c>
+      <c r="AC33">
+        <v>0</v>
+      </c>
+      <c r="AD33">
+        <v>0</v>
+      </c>
+      <c r="AE33">
+        <v>0</v>
+      </c>
+      <c r="AF33">
+        <v>0</v>
+      </c>
+      <c r="AG33">
+        <v>0</v>
+      </c>
+      <c r="AH33">
+        <v>0</v>
+      </c>
+      <c r="AI33">
+        <v>0</v>
+      </c>
+      <c r="AJ33">
+        <v>0</v>
+      </c>
+      <c r="AK33">
+        <v>0</v>
+      </c>
+      <c r="AL33">
+        <v>0</v>
+      </c>
+      <c r="AM33">
+        <v>0</v>
+      </c>
+      <c r="AN33">
+        <v>0</v>
+      </c>
+      <c r="AO33">
+        <v>0</v>
+      </c>
+      <c r="AP33">
+        <v>0</v>
+      </c>
+      <c r="AQ33">
+        <v>0</v>
+      </c>
+      <c r="AR33">
+        <v>0</v>
+      </c>
+      <c r="AS33">
+        <v>0</v>
+      </c>
+      <c r="AT33">
+        <v>0</v>
+      </c>
+      <c r="AU33">
+        <v>0</v>
+      </c>
+      <c r="AV33">
+        <v>0</v>
+      </c>
+      <c r="AW33">
+        <v>0</v>
+      </c>
+      <c r="AX33">
+        <v>0</v>
+      </c>
+      <c r="AY33">
+        <v>0</v>
+      </c>
+      <c r="AZ33">
+        <v>0</v>
+      </c>
+      <c r="BA33">
+        <v>0</v>
+      </c>
+      <c r="BB33">
+        <v>0</v>
+      </c>
+      <c r="BC33">
+        <v>0</v>
+      </c>
+      <c r="BD33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:56">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <v>0</v>
+      </c>
+      <c r="AB34">
+        <v>0</v>
+      </c>
+      <c r="AC34">
+        <v>0</v>
+      </c>
+      <c r="AD34">
+        <v>0</v>
+      </c>
+      <c r="AE34">
+        <v>0</v>
+      </c>
+      <c r="AF34">
+        <v>0</v>
+      </c>
+      <c r="AG34">
+        <v>0</v>
+      </c>
+      <c r="AH34">
+        <v>0</v>
+      </c>
+      <c r="AI34">
+        <v>0</v>
+      </c>
+      <c r="AJ34">
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <v>0</v>
+      </c>
+      <c r="AL34">
+        <v>0</v>
+      </c>
+      <c r="AM34">
+        <v>0</v>
+      </c>
+      <c r="AN34">
+        <v>0</v>
+      </c>
+      <c r="AO34">
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <v>0</v>
+      </c>
+      <c r="AQ34">
+        <v>0</v>
+      </c>
+      <c r="AR34">
+        <v>0</v>
+      </c>
+      <c r="AS34">
+        <v>0</v>
+      </c>
+      <c r="AT34">
+        <v>0</v>
+      </c>
+      <c r="AU34">
+        <v>0</v>
+      </c>
+      <c r="AV34">
+        <v>0</v>
+      </c>
+      <c r="AW34">
+        <v>0</v>
+      </c>
+      <c r="AX34">
+        <v>0</v>
+      </c>
+      <c r="AY34">
+        <v>0</v>
+      </c>
+      <c r="AZ34">
+        <v>0</v>
+      </c>
+      <c r="BA34">
+        <v>0</v>
+      </c>
+      <c r="BB34">
+        <v>0</v>
+      </c>
+      <c r="BC34">
+        <v>0</v>
+      </c>
+      <c r="BD34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:56">
+      <c r="A35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>0</v>
+      </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <v>0</v>
+      </c>
+      <c r="AB35">
+        <v>0</v>
+      </c>
+      <c r="AC35">
+        <v>0</v>
+      </c>
+      <c r="AD35">
+        <v>0</v>
+      </c>
+      <c r="AE35">
+        <v>0</v>
+      </c>
+      <c r="AF35">
+        <v>0</v>
+      </c>
+      <c r="AG35">
+        <v>0</v>
+      </c>
+      <c r="AH35">
+        <v>0</v>
+      </c>
+      <c r="AI35">
+        <v>0</v>
+      </c>
+      <c r="AJ35">
+        <v>0</v>
+      </c>
+      <c r="AK35">
+        <v>0</v>
+      </c>
+      <c r="AL35">
+        <v>0</v>
+      </c>
+      <c r="AM35">
+        <v>0</v>
+      </c>
+      <c r="AN35">
+        <v>0</v>
+      </c>
+      <c r="AO35">
+        <v>0</v>
+      </c>
+      <c r="AP35">
+        <v>0</v>
+      </c>
+      <c r="AQ35">
+        <v>0</v>
+      </c>
+      <c r="AR35">
+        <v>0</v>
+      </c>
+      <c r="AS35">
+        <v>0</v>
+      </c>
+      <c r="AT35">
+        <v>0</v>
+      </c>
+      <c r="AU35">
+        <v>0</v>
+      </c>
+      <c r="AV35">
+        <v>0</v>
+      </c>
+      <c r="AW35">
+        <v>0</v>
+      </c>
+      <c r="AX35">
+        <v>0</v>
+      </c>
+      <c r="AY35">
+        <v>0</v>
+      </c>
+      <c r="AZ35">
+        <v>0</v>
+      </c>
+      <c r="BA35">
+        <v>0</v>
+      </c>
+      <c r="BB35">
+        <v>0</v>
+      </c>
+      <c r="BC35">
+        <v>0</v>
+      </c>
+      <c r="BD35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:56">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>0</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <v>0</v>
+      </c>
+      <c r="AB36">
+        <v>0</v>
+      </c>
+      <c r="AC36">
+        <v>0</v>
+      </c>
+      <c r="AD36">
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <v>0</v>
+      </c>
+      <c r="AF36">
+        <v>0</v>
+      </c>
+      <c r="AG36">
+        <v>0</v>
+      </c>
+      <c r="AH36">
+        <v>0</v>
+      </c>
+      <c r="AI36">
+        <v>0</v>
+      </c>
+      <c r="AJ36">
+        <v>0</v>
+      </c>
+      <c r="AK36">
+        <v>0</v>
+      </c>
+      <c r="AL36">
+        <v>0</v>
+      </c>
+      <c r="AM36">
+        <v>0</v>
+      </c>
+      <c r="AN36">
+        <v>0</v>
+      </c>
+      <c r="AO36">
+        <v>0</v>
+      </c>
+      <c r="AP36">
+        <v>0</v>
+      </c>
+      <c r="AQ36">
+        <v>0</v>
+      </c>
+      <c r="AR36">
+        <v>0</v>
+      </c>
+      <c r="AS36">
+        <v>0</v>
+      </c>
+      <c r="AT36">
+        <v>0</v>
+      </c>
+      <c r="AU36">
+        <v>0</v>
+      </c>
+      <c r="AV36">
+        <v>0</v>
+      </c>
+      <c r="AW36">
+        <v>0</v>
+      </c>
+      <c r="AX36">
+        <v>0</v>
+      </c>
+      <c r="AY36">
+        <v>0</v>
+      </c>
+      <c r="AZ36">
+        <v>0</v>
+      </c>
+      <c r="BA36">
+        <v>0</v>
+      </c>
+      <c r="BB36">
+        <v>0</v>
+      </c>
+      <c r="BC36">
+        <v>0</v>
+      </c>
+      <c r="BD36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:56">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+      <c r="Y37">
+        <v>0</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37">
+        <v>0</v>
+      </c>
+      <c r="AB37">
+        <v>0</v>
+      </c>
+      <c r="AC37">
+        <v>0</v>
+      </c>
+      <c r="AD37">
+        <v>0</v>
+      </c>
+      <c r="AE37">
+        <v>0</v>
+      </c>
+      <c r="AF37">
+        <v>0</v>
+      </c>
+      <c r="AG37">
+        <v>0</v>
+      </c>
+      <c r="AH37">
+        <v>0</v>
+      </c>
+      <c r="AI37">
+        <v>0</v>
+      </c>
+      <c r="AJ37">
+        <v>0</v>
+      </c>
+      <c r="AK37">
+        <v>0</v>
+      </c>
+      <c r="AL37">
+        <v>0</v>
+      </c>
+      <c r="AM37">
+        <v>0</v>
+      </c>
+      <c r="AN37">
+        <v>0</v>
+      </c>
+      <c r="AO37">
+        <v>0</v>
+      </c>
+      <c r="AP37">
+        <v>0</v>
+      </c>
+      <c r="AQ37">
+        <v>0</v>
+      </c>
+      <c r="AR37">
+        <v>0</v>
+      </c>
+      <c r="AS37">
+        <v>0</v>
+      </c>
+      <c r="AT37">
+        <v>0</v>
+      </c>
+      <c r="AU37">
+        <v>0</v>
+      </c>
+      <c r="AV37">
+        <v>0</v>
+      </c>
+      <c r="AW37">
+        <v>0</v>
+      </c>
+      <c r="AX37">
+        <v>0</v>
+      </c>
+      <c r="AY37">
+        <v>0</v>
+      </c>
+      <c r="AZ37">
+        <v>0</v>
+      </c>
+      <c r="BA37">
+        <v>0</v>
+      </c>
+      <c r="BB37">
+        <v>0</v>
+      </c>
+      <c r="BC37">
+        <v>0</v>
+      </c>
+      <c r="BD37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:56">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <v>0</v>
+      </c>
+      <c r="Y38">
+        <v>0</v>
+      </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
+      <c r="AA38">
+        <v>0</v>
+      </c>
+      <c r="AB38">
+        <v>0</v>
+      </c>
+      <c r="AC38">
+        <v>0</v>
+      </c>
+      <c r="AD38">
+        <v>0</v>
+      </c>
+      <c r="AE38">
+        <v>0</v>
+      </c>
+      <c r="AF38">
+        <v>0</v>
+      </c>
+      <c r="AG38">
+        <v>0</v>
+      </c>
+      <c r="AH38">
+        <v>0</v>
+      </c>
+      <c r="AI38">
+        <v>0</v>
+      </c>
+      <c r="AJ38">
+        <v>0</v>
+      </c>
+      <c r="AK38">
+        <v>0</v>
+      </c>
+      <c r="AL38">
+        <v>0</v>
+      </c>
+      <c r="AM38">
+        <v>0</v>
+      </c>
+      <c r="AN38">
+        <v>0</v>
+      </c>
+      <c r="AO38">
+        <v>0</v>
+      </c>
+      <c r="AP38">
+        <v>0</v>
+      </c>
+      <c r="AQ38">
+        <v>0</v>
+      </c>
+      <c r="AR38">
+        <v>0</v>
+      </c>
+      <c r="AS38">
+        <v>0</v>
+      </c>
+      <c r="AT38">
+        <v>0</v>
+      </c>
+      <c r="AU38">
+        <v>0</v>
+      </c>
+      <c r="AV38">
+        <v>0</v>
+      </c>
+      <c r="AW38">
+        <v>0</v>
+      </c>
+      <c r="AX38">
+        <v>0</v>
+      </c>
+      <c r="AY38">
+        <v>0</v>
+      </c>
+      <c r="AZ38">
+        <v>0</v>
+      </c>
+      <c r="BA38">
+        <v>0</v>
+      </c>
+      <c r="BB38">
+        <v>0</v>
+      </c>
+      <c r="BC38">
+        <v>0</v>
+      </c>
+      <c r="BD38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:56">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+      <c r="X39">
+        <v>0</v>
+      </c>
+      <c r="Y39">
+        <v>0</v>
+      </c>
+      <c r="Z39">
+        <v>0</v>
+      </c>
+      <c r="AA39">
+        <v>0</v>
+      </c>
+      <c r="AB39">
+        <v>0</v>
+      </c>
+      <c r="AC39">
+        <v>0</v>
+      </c>
+      <c r="AD39">
+        <v>0</v>
+      </c>
+      <c r="AE39">
+        <v>0</v>
+      </c>
+      <c r="AF39">
+        <v>0</v>
+      </c>
+      <c r="AG39">
+        <v>0</v>
+      </c>
+      <c r="AH39">
+        <v>0</v>
+      </c>
+      <c r="AI39">
+        <v>0</v>
+      </c>
+      <c r="AJ39">
+        <v>0</v>
+      </c>
+      <c r="AK39">
+        <v>0</v>
+      </c>
+      <c r="AL39">
+        <v>0</v>
+      </c>
+      <c r="AM39">
+        <v>0</v>
+      </c>
+      <c r="AN39">
+        <v>0</v>
+      </c>
+      <c r="AO39">
+        <v>0</v>
+      </c>
+      <c r="AP39">
+        <v>0</v>
+      </c>
+      <c r="AQ39">
+        <v>0</v>
+      </c>
+      <c r="AR39">
+        <v>0</v>
+      </c>
+      <c r="AS39">
+        <v>0</v>
+      </c>
+      <c r="AT39">
+        <v>0</v>
+      </c>
+      <c r="AU39">
+        <v>0</v>
+      </c>
+      <c r="AV39">
+        <v>0</v>
+      </c>
+      <c r="AW39">
+        <v>0</v>
+      </c>
+      <c r="AX39">
+        <v>0</v>
+      </c>
+      <c r="AY39">
+        <v>0</v>
+      </c>
+      <c r="AZ39">
+        <v>0</v>
+      </c>
+      <c r="BA39">
+        <v>0</v>
+      </c>
+      <c r="BB39">
+        <v>0</v>
+      </c>
+      <c r="BC39">
+        <v>0</v>
+      </c>
+      <c r="BD39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:56">
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>0</v>
+      </c>
+      <c r="X40">
+        <v>0</v>
+      </c>
+      <c r="Y40">
+        <v>0</v>
+      </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
+      <c r="AA40">
+        <v>0</v>
+      </c>
+      <c r="AB40">
+        <v>0</v>
+      </c>
+      <c r="AC40">
+        <v>0</v>
+      </c>
+      <c r="AD40">
+        <v>0</v>
+      </c>
+      <c r="AE40">
+        <v>0</v>
+      </c>
+      <c r="AF40">
+        <v>0</v>
+      </c>
+      <c r="AG40">
+        <v>0</v>
+      </c>
+      <c r="AH40">
+        <v>0</v>
+      </c>
+      <c r="AI40">
+        <v>0</v>
+      </c>
+      <c r="AJ40">
+        <v>0</v>
+      </c>
+      <c r="AK40">
+        <v>0</v>
+      </c>
+      <c r="AL40">
+        <v>0</v>
+      </c>
+      <c r="AM40">
+        <v>0</v>
+      </c>
+      <c r="AN40">
+        <v>0</v>
+      </c>
+      <c r="AO40">
+        <v>0</v>
+      </c>
+      <c r="AP40">
+        <v>0</v>
+      </c>
+      <c r="AQ40">
+        <v>0</v>
+      </c>
+      <c r="AR40">
+        <v>0</v>
+      </c>
+      <c r="AS40">
+        <v>0</v>
+      </c>
+      <c r="AT40">
+        <v>0</v>
+      </c>
+      <c r="AU40">
+        <v>0</v>
+      </c>
+      <c r="AV40">
+        <v>0</v>
+      </c>
+      <c r="AW40">
+        <v>0</v>
+      </c>
+      <c r="AX40">
+        <v>0</v>
+      </c>
+      <c r="AY40">
+        <v>0</v>
+      </c>
+      <c r="AZ40">
+        <v>0</v>
+      </c>
+      <c r="BA40">
+        <v>0</v>
+      </c>
+      <c r="BB40">
+        <v>0</v>
+      </c>
+      <c r="BC40">
+        <v>0</v>
+      </c>
+      <c r="BD40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:56">
+      <c r="A41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>0</v>
+      </c>
+      <c r="X41">
+        <v>0</v>
+      </c>
+      <c r="Y41">
+        <v>0</v>
+      </c>
+      <c r="Z41">
+        <v>0</v>
+      </c>
+      <c r="AA41">
+        <v>0</v>
+      </c>
+      <c r="AB41">
+        <v>0</v>
+      </c>
+      <c r="AC41">
+        <v>0</v>
+      </c>
+      <c r="AD41">
+        <v>0</v>
+      </c>
+      <c r="AE41">
+        <v>0</v>
+      </c>
+      <c r="AF41">
+        <v>0</v>
+      </c>
+      <c r="AG41">
+        <v>0</v>
+      </c>
+      <c r="AH41">
+        <v>0</v>
+      </c>
+      <c r="AI41">
+        <v>0</v>
+      </c>
+      <c r="AJ41">
+        <v>0</v>
+      </c>
+      <c r="AK41">
+        <v>0</v>
+      </c>
+      <c r="AL41">
+        <v>0</v>
+      </c>
+      <c r="AM41">
+        <v>0</v>
+      </c>
+      <c r="AN41">
+        <v>0</v>
+      </c>
+      <c r="AO41">
+        <v>0</v>
+      </c>
+      <c r="AP41">
+        <v>0</v>
+      </c>
+      <c r="AQ41">
+        <v>0</v>
+      </c>
+      <c r="AR41">
+        <v>0</v>
+      </c>
+      <c r="AS41">
+        <v>0</v>
+      </c>
+      <c r="AT41">
+        <v>0</v>
+      </c>
+      <c r="AU41">
+        <v>0</v>
+      </c>
+      <c r="AV41">
+        <v>0</v>
+      </c>
+      <c r="AW41">
+        <v>0</v>
+      </c>
+      <c r="AX41">
+        <v>0</v>
+      </c>
+      <c r="AY41">
+        <v>0</v>
+      </c>
+      <c r="AZ41">
+        <v>0</v>
+      </c>
+      <c r="BA41">
+        <v>0</v>
+      </c>
+      <c r="BB41">
+        <v>0</v>
+      </c>
+      <c r="BC41">
+        <v>0</v>
+      </c>
+      <c r="BD41">
         <v>0</v>
       </c>
     </row>
@@ -6404,18 +8481,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" ht="12.6" spans="1:2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -6423,7 +8500,7 @@
     </row>
     <row r="3" ht="12.6" spans="1:2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -6431,7 +8508,7 @@
     </row>
     <row r="4" ht="12.6" spans="1:2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -6439,7 +8516,7 @@
     </row>
     <row r="5" ht="12.6" spans="1:2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -6447,7 +8524,7 @@
     </row>
     <row r="6" ht="12.6" spans="1:2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -6455,7 +8532,7 @@
     </row>
     <row r="7" ht="12.6" spans="1:2">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -6463,7 +8540,7 @@
     </row>
     <row r="8" ht="12.6" spans="1:2">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -6471,18 +8548,18 @@
     </row>
     <row r="9" ht="12.6" spans="1:3">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" ht="12.6" spans="1:2">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -6490,7 +8567,7 @@
     </row>
     <row r="11" ht="12.6" spans="1:2">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -6498,7 +8575,7 @@
     </row>
     <row r="12" ht="12.6" spans="1:2">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -6506,7 +8583,7 @@
     </row>
     <row r="13" ht="12.6" spans="1:2">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
@@ -6514,7 +8591,7 @@
     </row>
     <row r="14" ht="12.6" spans="1:2">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -6522,7 +8599,7 @@
     </row>
     <row r="15" ht="12.6" spans="1:2">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -6530,7 +8607,7 @@
     </row>
     <row r="16" ht="12.6" spans="1:2">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -6538,18 +8615,18 @@
     </row>
     <row r="17" ht="12.6" spans="1:3">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" ht="12.6" spans="1:2">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -6557,7 +8634,7 @@
     </row>
     <row r="19" ht="12.6" spans="1:2">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -6565,7 +8642,7 @@
     </row>
     <row r="20" ht="12.6" spans="1:2">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -6573,7 +8650,7 @@
     </row>
     <row r="21" ht="12.6" spans="1:2">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
@@ -6581,7 +8658,7 @@
     </row>
     <row r="22" ht="12.6" spans="1:2">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -6589,7 +8666,7 @@
     </row>
     <row r="23" ht="12.6" spans="1:2">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
@@ -6597,7 +8674,7 @@
     </row>
     <row r="24" ht="12.6" spans="1:2">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
@@ -6605,18 +8682,18 @@
     </row>
     <row r="25" ht="12.6" spans="1:3">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" ht="12.6" spans="1:2">
       <c r="A26" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -6624,7 +8701,7 @@
     </row>
     <row r="27" ht="12.6" spans="1:2">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -6632,7 +8709,7 @@
     </row>
     <row r="28" ht="12.6" spans="1:2">
       <c r="A28" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
@@ -6640,7 +8717,7 @@
     </row>
     <row r="29" ht="12.6" spans="1:2">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
@@ -6648,7 +8725,7 @@
     </row>
     <row r="30" ht="12.6" spans="1:2">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -6656,7 +8733,7 @@
     </row>
     <row r="31" ht="12.6" spans="1:2">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -6664,7 +8741,7 @@
     </row>
     <row r="32" ht="12.6" spans="1:2">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
@@ -6672,18 +8749,18 @@
     </row>
     <row r="33" ht="12.6" spans="1:3">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B33" t="s">
         <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" ht="12.6" spans="1:2">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
@@ -6691,7 +8768,7 @@
     </row>
     <row r="35" ht="12.6" spans="1:2">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
@@ -6699,7 +8776,7 @@
     </row>
     <row r="36" ht="12.6" spans="1:2">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
@@ -6707,7 +8784,7 @@
     </row>
     <row r="37" ht="12.6" spans="1:2">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -6715,7 +8792,7 @@
     </row>
     <row r="38" ht="12.6" spans="1:2">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
@@ -6723,7 +8800,7 @@
     </row>
     <row r="39" ht="12.6" spans="1:2">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
@@ -6731,7 +8808,7 @@
     </row>
     <row r="40" ht="12.6" spans="1:2">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="B40" t="s">
         <v>38</v>
@@ -6739,18 +8816,18 @@
     </row>
     <row r="41" ht="12.6" spans="1:3">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="B41" t="s">
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" ht="12.6" spans="1:2">
       <c r="A42" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="B42" t="s">
         <v>40</v>
@@ -6758,7 +8835,7 @@
     </row>
     <row r="43" ht="12.6" spans="1:2">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B43" t="s">
         <v>41</v>
@@ -6766,7 +8843,7 @@
     </row>
     <row r="44" ht="12.6" spans="1:2">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="B44" t="s">
         <v>42</v>
@@ -6774,7 +8851,7 @@
     </row>
     <row r="45" ht="12.6" spans="1:2">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="B45" t="s">
         <v>43</v>
@@ -6782,7 +8859,7 @@
     </row>
     <row r="46" ht="12.6" spans="1:2">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="B46" t="s">
         <v>44</v>
@@ -6790,7 +8867,7 @@
     </row>
     <row r="47" ht="12.6" spans="1:2">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s">
         <v>45</v>
@@ -6798,7 +8875,7 @@
     </row>
     <row r="48" ht="12.6" spans="1:2">
       <c r="A48" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
@@ -6806,18 +8883,18 @@
     </row>
     <row r="49" ht="12.6" spans="1:3">
       <c r="A49" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="B49" t="s">
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" ht="12.6" spans="1:2">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B50" t="s">
         <v>48</v>
@@ -6825,7 +8902,7 @@
     </row>
     <row r="51" ht="12.6" spans="1:2">
       <c r="A51" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
@@ -6833,7 +8910,7 @@
     </row>
     <row r="52" ht="12.6" spans="1:2">
       <c r="A52" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="B52" t="s">
         <v>50</v>
@@ -6841,7 +8918,7 @@
     </row>
     <row r="53" ht="12.6" spans="1:2">
       <c r="A53" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
         <v>51</v>
@@ -6849,7 +8926,7 @@
     </row>
     <row r="54" ht="12.6" spans="1:2">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
@@ -6857,7 +8934,7 @@
     </row>
     <row r="55" ht="12.6" spans="1:2">
       <c r="A55" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="B55" t="s">
         <v>53</v>
@@ -6865,7 +8942,7 @@
     </row>
     <row r="56" ht="12.6" spans="1:2">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Set default warm offset to 550
</commit_message>
<xml_diff>
--- a/data/default_biases_warm.xlsx
+++ b/data/default_biases_warm.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\zec\striptease\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BC6F11-87DA-4BA1-8A65-0726FC518D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9168"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Biases" sheetId="1" r:id="rId1"/>
     <sheet name="Modules" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Biases"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Modules"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -506,14 +512,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -539,353 +539,16 @@
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -893,318 +556,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+  <cellStyles count="1">
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1462,26 +839,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:BD41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:XFC41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:BD41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34:BD37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.8888888888889" style="1" customWidth="1"/>
-    <col min="2" max="1021" width="8.5462962962963" style="1" customWidth="1"/>
-    <col min="1022" max="1022" width="11.5185185185185" style="1" customWidth="1"/>
-    <col min="1023" max="1024" width="9.13888888888889" style="1" customWidth="1"/>
-    <col min="1025" max="16383" width="9.13888888888889" style="1"/>
-    <col min="16384" max="16384" width="9.13888888888889"/>
+    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
+    <col min="2" max="1021" width="8.5703125" style="1" customWidth="1"/>
+    <col min="1022" max="1022" width="11.5703125" style="1" customWidth="1"/>
+    <col min="1023" max="1024" width="9.140625" style="1" customWidth="1"/>
+    <col min="1025" max="16383" width="9.140625" style="1"/>
+    <col min="16384" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56">
@@ -5441,7 +4821,7 @@
         <v>4738.96</v>
       </c>
       <c r="P24">
-        <v>4560.4</v>
+        <v>4560.3999999999996</v>
       </c>
       <c r="Q24" s="3">
         <v>11732.56</v>
@@ -5459,7 +4839,7 @@
         <v>3498.96</v>
       </c>
       <c r="V24">
-        <v>5046.48</v>
+        <v>5046.4799999999996</v>
       </c>
       <c r="W24">
         <v>7556.24</v>
@@ -5519,7 +4899,7 @@
         <v>8518.48</v>
       </c>
       <c r="AP24">
-        <v>2219.28</v>
+        <v>2219.2800000000002</v>
       </c>
       <c r="AQ24">
         <v>2318.48</v>
@@ -5534,7 +4914,7 @@
         <v>5453.2</v>
       </c>
       <c r="AU24">
-        <v>542.8</v>
+        <v>542.79999999999995</v>
       </c>
       <c r="AV24" s="3">
         <v>10234.64</v>
@@ -5614,7 +4994,7 @@
         <v>6822.16</v>
       </c>
       <c r="Q25" s="3">
-        <v>21979.92</v>
+        <v>21979.919999999998</v>
       </c>
       <c r="R25">
         <v>4719.12</v>
@@ -5647,7 +5027,7 @@
         <v>10869.52</v>
       </c>
       <c r="AB25">
-        <v>8945.04</v>
+        <v>8945.0400000000009</v>
       </c>
       <c r="AC25">
         <v>3727.12</v>
@@ -5683,7 +5063,7 @@
         <v>7962.96</v>
       </c>
       <c r="AN25" s="3">
-        <v>8706.96</v>
+        <v>8706.9599999999991</v>
       </c>
       <c r="AO25">
         <v>4967.12</v>
@@ -5716,7 +5096,7 @@
         <v>5701.2</v>
       </c>
       <c r="AY25">
-        <v>4282.64</v>
+        <v>4282.6400000000003</v>
       </c>
       <c r="AZ25">
         <v>2020.88</v>
@@ -5754,7 +5134,7 @@
         <v>4094.16</v>
       </c>
       <c r="G26">
-        <v>4808.4</v>
+        <v>4808.3999999999996</v>
       </c>
       <c r="H26">
         <v>14272.08</v>
@@ -5787,7 +5167,7 @@
         <v>-82.16</v>
       </c>
       <c r="R26">
-        <v>4689.36</v>
+        <v>4689.3599999999997</v>
       </c>
       <c r="S26">
         <v>2506.96</v>
@@ -5811,7 +5191,7 @@
         <v>0</v>
       </c>
       <c r="Z26">
-        <v>5175.44</v>
+        <v>5175.4399999999996</v>
       </c>
       <c r="AA26">
         <v>9371.6</v>
@@ -5826,7 +5206,7 @@
         <v>3072.4</v>
       </c>
       <c r="AE26">
-        <v>4937.36</v>
+        <v>4937.3599999999997</v>
       </c>
       <c r="AF26">
         <v>8597.84</v>
@@ -5844,7 +5224,7 @@
         <v>3022.8</v>
       </c>
       <c r="AK26">
-        <v>4550.48</v>
+        <v>4550.4799999999996</v>
       </c>
       <c r="AL26">
         <v>3568.4</v>
@@ -5856,7 +5236,7 @@
         <v>0</v>
       </c>
       <c r="AO26">
-        <v>8954.96</v>
+        <v>8954.9599999999991</v>
       </c>
       <c r="AP26">
         <v>8607.76</v>
@@ -5889,7 +5269,7 @@
         <v>3459.28</v>
       </c>
       <c r="AZ26">
-        <v>9956.88</v>
+        <v>9956.8799999999992</v>
       </c>
       <c r="BA26">
         <v>5602</v>
@@ -5921,7 +5301,7 @@
         <v>6554.32</v>
       </c>
       <c r="F27">
-        <v>4431.44</v>
+        <v>4431.4399999999996</v>
       </c>
       <c r="G27">
         <v>4947.28</v>
@@ -5936,7 +5316,7 @@
         <v>11008.4</v>
       </c>
       <c r="K27">
-        <v>4917.52</v>
+        <v>4917.5200000000004</v>
       </c>
       <c r="L27">
         <v>6931.28</v>
@@ -5999,7 +5379,7 @@
         <v>5225.04</v>
       </c>
       <c r="AF27">
-        <v>4937.36</v>
+        <v>4937.3599999999997</v>
       </c>
       <c r="AG27">
         <v>3151.76</v>
@@ -6041,7 +5421,7 @@
         <v>3707.28</v>
       </c>
       <c r="AT27">
-        <v>9202.96</v>
+        <v>9202.9599999999991</v>
       </c>
       <c r="AU27">
         <v>6256.72</v>
@@ -6082,7 +5462,7 @@
         <v>6177.36</v>
       </c>
       <c r="C28">
-        <v>4808.4</v>
+        <v>4808.3999999999996</v>
       </c>
       <c r="D28">
         <v>5096.08</v>
@@ -6094,7 +5474,7 @@
         <v>4252.88</v>
       </c>
       <c r="G28">
-        <v>4183.44</v>
+        <v>4183.4399999999996</v>
       </c>
       <c r="H28">
         <v>1733.2</v>
@@ -6103,13 +5483,13 @@
         <v>16216.4</v>
       </c>
       <c r="J28">
-        <v>4193.36</v>
+        <v>4193.3599999999997</v>
       </c>
       <c r="K28">
         <v>4709.2</v>
       </c>
       <c r="L28">
-        <v>2467.28</v>
+        <v>2467.2800000000002</v>
       </c>
       <c r="M28">
         <v>7605.84</v>
@@ -6124,10 +5504,10 @@
         <v>6643.6</v>
       </c>
       <c r="Q28" s="3">
-        <v>23596.88</v>
+        <v>23596.880000000001</v>
       </c>
       <c r="R28">
-        <v>4173.52</v>
+        <v>4173.5200000000004</v>
       </c>
       <c r="S28">
         <v>7834</v>
@@ -6148,16 +5528,16 @@
         <v>6197.2</v>
       </c>
       <c r="Y28" s="3">
-        <v>17972.24</v>
+        <v>17972.240000000002</v>
       </c>
       <c r="Z28">
         <v>2943.44</v>
       </c>
       <c r="AA28">
-        <v>9689.04</v>
+        <v>9689.0400000000009</v>
       </c>
       <c r="AB28">
-        <v>4431.44</v>
+        <v>4431.4399999999996</v>
       </c>
       <c r="AC28">
         <v>4500.88</v>
@@ -6202,7 +5582,7 @@
         <v>6107.92</v>
       </c>
       <c r="AQ28">
-        <v>4530.64</v>
+        <v>4530.6400000000003</v>
       </c>
       <c r="AR28">
         <v>9262.48</v>
@@ -6321,7 +5701,7 @@
         <v>13379.28</v>
       </c>
       <c r="Z29">
-        <v>2536.72</v>
+        <v>2536.7199999999998</v>
       </c>
       <c r="AA29">
         <v>10135.44</v>
@@ -6354,16 +5734,16 @@
         <v>7843.92</v>
       </c>
       <c r="AK29">
-        <v>4441.36</v>
+        <v>4441.3599999999997</v>
       </c>
       <c r="AL29">
         <v>3370</v>
       </c>
       <c r="AM29">
-        <v>4431.44</v>
+        <v>4431.4399999999996</v>
       </c>
       <c r="AN29" s="3">
-        <v>5175.44</v>
+        <v>5175.4399999999996</v>
       </c>
       <c r="AO29">
         <v>7764.56</v>
@@ -6375,13 +5755,13 @@
         <v>3727.12</v>
       </c>
       <c r="AR29">
-        <v>9450.96</v>
+        <v>9450.9599999999991</v>
       </c>
       <c r="AS29">
         <v>3796.56</v>
       </c>
       <c r="AT29">
-        <v>5155.6</v>
+        <v>5155.6000000000004</v>
       </c>
       <c r="AU29">
         <v>3270.8</v>
@@ -7099,169 +6479,169 @@
         <v>88</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="L34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="M34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="N34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="O34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="P34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Q34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="R34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="S34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="T34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="U34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="V34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="W34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="X34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Y34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Z34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AA34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AB34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AC34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AD34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AE34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AF34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AG34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AH34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AI34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AJ34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AK34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AL34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AM34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AN34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AO34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AP34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AQ34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AR34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AS34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AT34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AU34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AV34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AW34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AX34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AY34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AZ34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BA34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BB34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BC34">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BD34">
-        <v>0</v>
+        <v>550</v>
       </c>
     </row>
     <row r="35" spans="1:56">
@@ -7269,169 +6649,169 @@
         <v>89</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="K35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="L35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="M35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="N35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="O35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="P35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Q35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="R35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="S35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="T35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="U35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="V35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="W35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="X35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Y35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Z35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AA35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AB35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AC35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AD35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AE35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AF35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AG35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AH35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AI35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AJ35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AK35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AL35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AM35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AN35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AO35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AP35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AQ35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AR35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AS35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AT35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AU35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AV35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AW35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AX35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AY35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AZ35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BA35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BB35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BC35">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BD35">
-        <v>0</v>
+        <v>550</v>
       </c>
     </row>
     <row r="36" spans="1:56">
@@ -7439,169 +6819,169 @@
         <v>90</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="K36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="L36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="M36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="N36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="O36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="P36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Q36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="R36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="S36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="T36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="U36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="V36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="W36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="X36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Y36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Z36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AA36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AB36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AC36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AD36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AE36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AF36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AG36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AH36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AI36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AJ36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AK36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AL36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AM36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AN36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AO36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AP36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AQ36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AR36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AS36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AT36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AU36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AV36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AW36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AX36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AY36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AZ36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BA36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BB36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BC36">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BD36">
-        <v>0</v>
+        <v>550</v>
       </c>
     </row>
     <row r="37" spans="1:56">
@@ -7609,169 +6989,169 @@
         <v>91</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="K37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="L37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="M37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="N37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="O37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="P37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Q37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="R37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="S37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="T37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="U37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="V37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="W37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="X37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Y37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="Z37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AA37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AB37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AC37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AD37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AE37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AF37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AG37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AH37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AI37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AJ37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AK37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AL37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AM37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AN37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AO37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AP37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AQ37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AR37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AS37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AT37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AU37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AV37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AW37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AX37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AY37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AZ37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BA37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BB37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BC37">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="BD37">
-        <v>0</v>
+        <v>550</v>
       </c>
     </row>
     <row r="38" spans="1:56">
@@ -8455,28 +7835,26 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.83333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1111111111111" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="8.5462962962963" style="1" customWidth="1"/>
-    <col min="1026" max="16384" width="9.13888888888889" style="1"/>
+    <col min="1" max="1" width="7.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="8.5703125" style="1" customWidth="1"/>
+    <col min="1026" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -8490,7 +7868,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" ht="12.6" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -8498,7 +7876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="12.6" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -8506,7 +7884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" ht="12.6" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -8514,7 +7892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" ht="12.6" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -8522,7 +7900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="12.6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -8530,7 +7908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" ht="12.6" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -8538,7 +7916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" ht="12.6" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -8546,7 +7924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" ht="12.6" spans="1:3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>106</v>
       </c>
@@ -8557,7 +7935,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" ht="12.6" spans="1:2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -8565,7 +7943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" ht="12.6" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -8573,7 +7951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" ht="12.6" spans="1:2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -8581,7 +7959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" ht="12.6" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>111</v>
       </c>
@@ -8589,7 +7967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" ht="12.6" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>112</v>
       </c>
@@ -8597,7 +7975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" ht="12.6" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>113</v>
       </c>
@@ -8605,7 +7983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" ht="12.6" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -8613,7 +7991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" ht="12.6" spans="1:3">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>115</v>
       </c>
@@ -8624,7 +8002,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" ht="12.6" spans="1:2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -8632,7 +8010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" ht="12.6" spans="1:2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>118</v>
       </c>
@@ -8640,7 +8018,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" ht="12.6" spans="1:2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -8648,7 +8026,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" ht="12.6" spans="1:2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>120</v>
       </c>
@@ -8656,7 +8034,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" ht="12.6" spans="1:2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>121</v>
       </c>
@@ -8664,7 +8042,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" ht="12.6" spans="1:2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -8672,7 +8050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" ht="12.6" spans="1:2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>123</v>
       </c>
@@ -8680,7 +8058,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" ht="12.6" spans="1:3">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -8691,7 +8069,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" ht="12.6" spans="1:2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>126</v>
       </c>
@@ -8699,7 +8077,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" ht="12.6" spans="1:2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>127</v>
       </c>
@@ -8707,7 +8085,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" ht="12.6" spans="1:2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>128</v>
       </c>
@@ -8715,7 +8093,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" ht="12.6" spans="1:2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>129</v>
       </c>
@@ -8723,7 +8101,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" ht="12.6" spans="1:2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>130</v>
       </c>
@@ -8731,7 +8109,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" ht="12.6" spans="1:2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>131</v>
       </c>
@@ -8739,7 +8117,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" ht="12.6" spans="1:2">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>132</v>
       </c>
@@ -8747,7 +8125,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" ht="12.6" spans="1:3">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>133</v>
       </c>
@@ -8758,7 +8136,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" ht="12.6" spans="1:2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>135</v>
       </c>
@@ -8766,7 +8144,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" ht="12.6" spans="1:2">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>136</v>
       </c>
@@ -8774,7 +8152,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" ht="12.6" spans="1:2">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>137</v>
       </c>
@@ -8782,7 +8160,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" ht="12.6" spans="1:2">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>138</v>
       </c>
@@ -8790,7 +8168,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" ht="12.6" spans="1:2">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>139</v>
       </c>
@@ -8798,7 +8176,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" ht="12.6" spans="1:2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>140</v>
       </c>
@@ -8806,7 +8184,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" ht="12.6" spans="1:2">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>141</v>
       </c>
@@ -8814,7 +8192,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" ht="12.6" spans="1:3">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>142</v>
       </c>
@@ -8825,7 +8203,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" ht="12.6" spans="1:2">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>144</v>
       </c>
@@ -8833,7 +8211,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" ht="12.6" spans="1:2">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>145</v>
       </c>
@@ -8841,7 +8219,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" ht="12.6" spans="1:2">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>146</v>
       </c>
@@ -8849,7 +8227,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" ht="12.6" spans="1:2">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>147</v>
       </c>
@@ -8857,7 +8235,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" ht="12.6" spans="1:2">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>148</v>
       </c>
@@ -8865,7 +8243,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" ht="12.6" spans="1:2">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>149</v>
       </c>
@@ -8873,7 +8251,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" ht="12.6" spans="1:2">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>150</v>
       </c>
@@ -8881,7 +8259,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" ht="12.6" spans="1:3">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>151</v>
       </c>
@@ -8892,7 +8270,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" ht="12.6" spans="1:2">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>153</v>
       </c>
@@ -8900,7 +8278,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" ht="12.6" spans="1:2">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>154</v>
       </c>
@@ -8908,7 +8286,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" ht="12.6" spans="1:2">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>155</v>
       </c>
@@ -8916,7 +8294,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" ht="12.6" spans="1:2">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>156</v>
       </c>
@@ -8924,7 +8302,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" ht="12.6" spans="1:2">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>157</v>
       </c>
@@ -8932,7 +8310,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" ht="12.6" spans="1:2">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>158</v>
       </c>
@@ -8940,7 +8318,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" ht="12.6" spans="1:2">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -8949,8 +8327,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;CTimes New Roman,Normale"2&amp;A</oddHeader>

</xml_diff>